<commit_message>
trying to revert back to before i messed it all up
</commit_message>
<xml_diff>
--- a/data/add-ons/add_factors_old_sophia.xlsx
+++ b/data/add-ons/add_factors_old_sophia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scampbell\Documents\GitHub\Fiscal-Impact-Measure\data\add-ons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B2CDF-1BDD-4301-B563-65227E2F3576}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C0502C-FC58-4492-A55D-4D6A183ED256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
@@ -66,7 +66,6 @@
     <author>tc={A0B72D47-4ADC-4971-B431-B9EA6C91AE60}</author>
     <author>tc={2D81BDF9-A0D8-4A1A-915B-91D32E8E61FF}</author>
     <author>tc={33EF6DF5-9556-47EC-86E1-A12FDBDC0AA8}</author>
-    <author>tc={40167970-C0F0-4C09-9098-80E03CD0CE14}</author>
     <author>tc={8D1CFFB8-D62F-4FA1-AB58-5320D39AA096}</author>
     <author>tc={DA48DE65-66E5-4DD8-819A-2F757A61D389}</author>
     <author>tc={1FC8F5D3-F5DD-4502-A8BF-AD36B99CFAF5}</author>
@@ -533,17 +532,7 @@
     we're comfortable leaving this as is</t>
       </text>
     </comment>
-    <comment ref="L78" authorId="15" shapeId="0" xr:uid="{40167970-C0F0-4C09-9098-80E03CD0CE14}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CBO indicated 17 for q2? why do we split the quarter 3 payments into q2?
-Reply:
-    we're comfortable leaving this as is</t>
-      </text>
-    </comment>
-    <comment ref="O82" authorId="16" shapeId="0" xr:uid="{8D1CFFB8-D62F-4FA1-AB58-5320D39AA096}">
+    <comment ref="O82" authorId="15" shapeId="0" xr:uid="{8D1CFFB8-D62F-4FA1-AB58-5320D39AA096}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -551,7 +540,7 @@
     CRFB estimates $29B ($45 minus $16B for airline which is inn subsidies). MPC is 100% over 12 quarters. And then annualized</t>
       </text>
     </comment>
-    <comment ref="O83" authorId="17" shapeId="0" xr:uid="{DA48DE65-66E5-4DD8-819A-2F757A61D389}">
+    <comment ref="O83" authorId="16" shapeId="0" xr:uid="{DA48DE65-66E5-4DD8-819A-2F757A61D389}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -559,7 +548,7 @@
     CRFB: estimates $82B. According to the Louise x Wendy, MPC is 100% over 3 years.</t>
       </text>
     </comment>
-    <comment ref="O84" authorId="18" shapeId="0" xr:uid="{1FC8F5D3-F5DD-4502-A8BF-AD36B99CFAF5}">
+    <comment ref="O84" authorId="17" shapeId="0" xr:uid="{1FC8F5D3-F5DD-4502-A8BF-AD36B99CFAF5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -567,7 +556,7 @@
     CRFB: estimates $63B. MPC is 100% over 12 quarters and then annualize</t>
       </text>
     </comment>
-    <comment ref="O85" authorId="19" shapeId="0" xr:uid="{99D44059-B7C8-4B13-A311-FD754252DDFC}">
+    <comment ref="O85" authorId="18" shapeId="0" xr:uid="{99D44059-B7C8-4B13-A311-FD754252DDFC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -600,7 +589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N101" authorId="20" shapeId="0" xr:uid="{11731043-8530-4DAC-9476-3C98D0D836BB}">
+    <comment ref="N101" authorId="19" shapeId="0" xr:uid="{11731043-8530-4DAC-9476-3C98D0D836BB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -641,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O113" authorId="21" shapeId="0" xr:uid="{D84F0053-F219-4B69-8181-0F12AE7D3FC2}">
+    <comment ref="O113" authorId="20" shapeId="0" xr:uid="{D84F0053-F219-4B69-8181-0F12AE7D3FC2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -651,7 +640,7 @@
     cbo proected it will be 2.3%. should we still ovverride with 4%?</t>
       </text>
     </comment>
-    <comment ref="P113" authorId="22" shapeId="0" xr:uid="{3B711313-D2C6-42FC-83C8-BA827015079B}">
+    <comment ref="P113" authorId="21" shapeId="0" xr:uid="{3B711313-D2C6-42FC-83C8-BA827015079B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2161,7 +2150,7 @@
     <numFmt numFmtId="171" formatCode="0.000%"/>
     <numFmt numFmtId="172" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2383,12 +2372,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3513,29 +3496,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="9" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3611,21 +3571,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3647,18 +3592,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="9" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4109,12 +4092,6 @@
   <threadedComment ref="L77" dT="2020-10-28T16:31:53.35" personId="{2D35AFA9-F227-4AE7-B9A7-D673D9D18C70}" id="{1079BF34-6E2F-4888-8715-72B28B28D9AA}" parentId="{33EF6DF5-9556-47EC-86E1-A12FDBDC0AA8}">
     <text>we're comfortable leaving this as is</text>
   </threadedComment>
-  <threadedComment ref="L78" dT="2020-10-27T15:26:37.39" personId="{2D35AFA9-F227-4AE7-B9A7-D673D9D18C70}" id="{40167970-C0F0-4C09-9098-80E03CD0CE14}">
-    <text>CBO indicated 17 for q2? why do we split the quarter 3 payments into q2?</text>
-  </threadedComment>
-  <threadedComment ref="L78" dT="2020-10-28T16:31:53.35" personId="{2D35AFA9-F227-4AE7-B9A7-D673D9D18C70}" id="{E1C08428-8D2F-4F91-B16A-33C4F07D6062}" parentId="{40167970-C0F0-4C09-9098-80E03CD0CE14}">
-    <text>we're comfortable leaving this as is</text>
-  </threadedComment>
   <threadedComment ref="O82" dT="2020-12-21T21:08:26.13" personId="{2D35AFA9-F227-4AE7-B9A7-D673D9D18C70}" id="{8D1CFFB8-D62F-4FA1-AB58-5320D39AA096}">
     <text>CRFB estimates $29B ($45 minus $16B for airline which is inn subsidies). MPC is 100% over 12 quarters. And then annualized</text>
   </threadedComment>
@@ -4202,86 +4179,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="342" t="s">
+      <c r="A1" s="327" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="342"/>
+      <c r="B1" s="327"/>
       <c r="C1" s="268"/>
       <c r="D1" s="268"/>
       <c r="E1" s="35"/>
       <c r="N1" t="s">
         <v>373</v>
       </c>
-      <c r="AC1" s="348" t="s">
+      <c r="AC1" s="333" t="s">
         <v>247</v>
       </c>
-      <c r="AD1" s="348"/>
-      <c r="AE1" s="346" t="s">
+      <c r="AD1" s="333"/>
+      <c r="AE1" s="331" t="s">
         <v>245</v>
       </c>
-      <c r="AF1" s="347"/>
+      <c r="AF1" s="332"/>
       <c r="AG1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="344" t="s">
+      <c r="AI1" s="329" t="s">
         <v>278</v>
       </c>
-      <c r="AJ1" s="344"/>
-      <c r="AK1" s="344"/>
-      <c r="AL1" s="344"/>
-      <c r="AM1" s="343" t="s">
+      <c r="AJ1" s="329"/>
+      <c r="AK1" s="329"/>
+      <c r="AL1" s="329"/>
+      <c r="AM1" s="328" t="s">
         <v>276</v>
       </c>
-      <c r="AN1" s="343"/>
-      <c r="AO1" s="343"/>
-      <c r="AP1" s="343"/>
+      <c r="AN1" s="328"/>
+      <c r="AO1" s="328"/>
+      <c r="AP1" s="328"/>
     </row>
     <row r="2" spans="1:43" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="341" t="s">
+      <c r="F2" s="326" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="341"/>
-      <c r="H2" s="341"/>
-      <c r="I2" s="341"/>
-      <c r="J2" s="341" t="s">
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
+      <c r="J2" s="326" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="341"/>
-      <c r="L2" s="341"/>
-      <c r="M2" s="341"/>
-      <c r="N2" s="341" t="s">
+      <c r="K2" s="326"/>
+      <c r="L2" s="326"/>
+      <c r="M2" s="326"/>
+      <c r="N2" s="326" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="341"/>
-      <c r="P2" s="341"/>
-      <c r="Q2" s="341"/>
-      <c r="R2" s="341" t="s">
+      <c r="O2" s="326"/>
+      <c r="P2" s="326"/>
+      <c r="Q2" s="326"/>
+      <c r="R2" s="326" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="341"/>
-      <c r="T2" s="341"/>
-      <c r="U2" s="341"/>
-      <c r="V2" s="341" t="s">
+      <c r="S2" s="326"/>
+      <c r="T2" s="326"/>
+      <c r="U2" s="326"/>
+      <c r="V2" s="326" t="s">
         <v>265</v>
       </c>
-      <c r="W2" s="341"/>
-      <c r="X2" s="341"/>
-      <c r="Y2" s="341"/>
+      <c r="W2" s="326"/>
+      <c r="X2" s="326"/>
+      <c r="Y2" s="326"/>
       <c r="Z2" s="221"/>
       <c r="AA2" s="283"/>
       <c r="AB2" s="221"/>
-      <c r="AC2" s="341" t="s">
+      <c r="AC2" s="326" t="s">
         <v>102</v>
       </c>
-      <c r="AD2" s="341"/>
-      <c r="AE2" s="341"/>
-      <c r="AF2" s="341"/>
-      <c r="AG2" s="341"/>
-      <c r="AH2" s="341"/>
-      <c r="AI2" s="341"/>
-      <c r="AJ2" s="341"/>
-      <c r="AK2" s="341"/>
-      <c r="AL2" s="345"/>
+      <c r="AD2" s="326"/>
+      <c r="AE2" s="326"/>
+      <c r="AF2" s="326"/>
+      <c r="AG2" s="326"/>
+      <c r="AH2" s="326"/>
+      <c r="AI2" s="326"/>
+      <c r="AJ2" s="326"/>
+      <c r="AK2" s="326"/>
+      <c r="AL2" s="330"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="F3" s="197" t="s">
@@ -4388,10 +4365,10 @@
       </c>
     </row>
     <row r="4" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="340" t="s">
+      <c r="A4" s="325" t="s">
         <v>261</v>
       </c>
-      <c r="B4" s="340"/>
+      <c r="B4" s="325"/>
       <c r="C4" s="268"/>
       <c r="D4" s="268"/>
       <c r="F4" s="197"/>
@@ -6416,31 +6393,31 @@
         <v>2925056</v>
       </c>
       <c r="O34" s="133">
-        <f t="shared" ref="O34:U34" si="29">O35+O40+O51</f>
+        <f>O35+O40+O51</f>
         <v>3270456.7169724014</v>
       </c>
       <c r="P34" s="133">
-        <f t="shared" si="29"/>
+        <f>P35+P40+P51</f>
         <v>2708796.7165770018</v>
       </c>
       <c r="Q34" s="133">
-        <f t="shared" si="29"/>
+        <f>Q35+Q40+Q51</f>
         <v>2611509.6718853824</v>
       </c>
       <c r="R34" s="133">
-        <f t="shared" si="29"/>
+        <f>R35+R40+R51</f>
         <v>2678465.9441347551</v>
       </c>
       <c r="S34" s="133">
-        <f t="shared" si="29"/>
+        <f>S35+S40+S51</f>
         <v>2735176.6542439447</v>
       </c>
       <c r="T34" s="133">
-        <f t="shared" si="29"/>
+        <f>T35+T40+T51</f>
         <v>2793300.2519227522</v>
       </c>
       <c r="U34" s="133">
-        <f t="shared" si="29"/>
+        <f>U35+U40+U51</f>
         <v>2852876.3150512893</v>
       </c>
       <c r="V34" s="87"/>
@@ -6818,35 +6795,35 @@
         <v>338269</v>
       </c>
       <c r="O40" s="87">
-        <f t="shared" ref="O40:V40" si="30">O42+O46</f>
+        <f t="shared" ref="O40:V40" si="29">O42+O46</f>
         <v>724000</v>
       </c>
       <c r="P40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>152000</v>
       </c>
       <c r="Q40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="R40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="S40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="T40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="U40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="V40" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>44000</v>
       </c>
       <c r="W40" s="44"/>
@@ -6868,7 +6845,7 @@
         <v>314.56725</v>
       </c>
       <c r="AF40" s="45">
-        <f t="shared" ref="AF40:AF51" si="31">AVERAGE(R40:U40)/1000</f>
+        <f t="shared" ref="AF40:AF51" si="30">AVERAGE(R40:U40)/1000</f>
         <v>44</v>
       </c>
       <c r="AH40">
@@ -6967,11 +6944,11 @@
         <v>108000</v>
       </c>
       <c r="Q42" s="87">
-        <f t="shared" ref="Q42" si="32">Q43+Q44+Q45</f>
+        <f t="shared" ref="Q42" si="31">Q43+Q44+Q45</f>
         <v>0</v>
       </c>
       <c r="R42" s="87">
-        <f t="shared" ref="R42" si="33">R43+R44</f>
+        <f t="shared" ref="R42" si="32">R43+R44</f>
         <v>0</v>
       </c>
       <c r="S42" s="87"/>
@@ -7065,7 +7042,7 @@
         <v>139.42500000000001</v>
       </c>
       <c r="AF43" s="45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AG43" s="3"/>
@@ -7231,7 +7208,7 @@
         <v>46.174999999999997</v>
       </c>
       <c r="AF46" s="45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>44</v>
       </c>
       <c r="AG46" s="3"/>
@@ -7242,81 +7219,81 @@
       <c r="AM46" s="182"/>
     </row>
     <row r="47" spans="1:39" s="107" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="325" t="s">
+      <c r="A47" s="368" t="s">
         <v>147</v>
       </c>
-      <c r="F47" s="326"/>
-      <c r="G47" s="326"/>
-      <c r="H47" s="326"/>
-      <c r="I47" s="326"/>
-      <c r="J47" s="326">
+      <c r="F47" s="369"/>
+      <c r="G47" s="369"/>
+      <c r="H47" s="369"/>
+      <c r="I47" s="369"/>
+      <c r="J47" s="369">
         <v>0</v>
       </c>
-      <c r="K47" s="326">
+      <c r="K47" s="369">
         <v>0</v>
       </c>
-      <c r="L47" s="326">
+      <c r="L47" s="369">
         <f>SUM(L48:L50)</f>
         <v>179900</v>
       </c>
-      <c r="M47" s="327">
+      <c r="M47" s="370">
         <v>85400</v>
       </c>
-      <c r="N47" s="328">
+      <c r="N47" s="371">
         <f>SUM(N48:N50)</f>
         <v>45300</v>
       </c>
-      <c r="O47" s="329">
-        <f t="shared" ref="O47:R47" si="34">SUM(O48:O50)</f>
+      <c r="O47" s="372">
+        <f t="shared" ref="O47:R47" si="33">SUM(O48:O50)</f>
         <v>54177.595548489669</v>
       </c>
-      <c r="P47" s="329">
-        <f t="shared" si="34"/>
+      <c r="P47" s="372">
+        <f t="shared" si="33"/>
         <v>43000</v>
       </c>
-      <c r="Q47" s="329">
-        <f t="shared" si="34"/>
+      <c r="Q47" s="372">
+        <f t="shared" si="33"/>
         <v>43000</v>
       </c>
-      <c r="R47" s="329">
-        <f t="shared" si="34"/>
+      <c r="R47" s="372">
+        <f t="shared" si="33"/>
         <v>15000</v>
       </c>
-      <c r="S47" s="329"/>
-      <c r="T47" s="329"/>
-      <c r="U47" s="329"/>
-      <c r="V47" s="330"/>
-      <c r="W47" s="330"/>
-      <c r="X47" s="330"/>
-      <c r="Y47" s="330"/>
-      <c r="Z47" s="330"/>
-      <c r="AA47" s="330"/>
-      <c r="AB47" s="330"/>
-      <c r="AC47" s="330"/>
-      <c r="AD47" s="331">
+      <c r="S47" s="372"/>
+      <c r="T47" s="372"/>
+      <c r="U47" s="372"/>
+      <c r="V47" s="373"/>
+      <c r="W47" s="373"/>
+      <c r="X47" s="373"/>
+      <c r="Y47" s="373"/>
+      <c r="Z47" s="373"/>
+      <c r="AA47" s="373"/>
+      <c r="AB47" s="373"/>
+      <c r="AC47" s="373"/>
+      <c r="AD47" s="374">
         <f>AVERAGE(J47:M47)/1000</f>
         <v>66.325000000000003</v>
       </c>
-      <c r="AE47" s="331">
+      <c r="AE47" s="374">
         <f>AVERAGE(N47:Q47)/1000</f>
         <v>46.369398887122415</v>
       </c>
-      <c r="AF47" s="331">
-        <f t="shared" ref="AF47" si="35">AVERAGE(R47:U47)/1000</f>
+      <c r="AF47" s="374">
+        <f t="shared" ref="AF47" si="34">AVERAGE(R47:U47)/1000</f>
         <v>15</v>
       </c>
-      <c r="AG47" s="330"/>
-      <c r="AI47" s="330">
+      <c r="AG47" s="373"/>
+      <c r="AI47" s="373">
         <f>'figuring out social benefits'!G48</f>
         <v>105</v>
       </c>
-      <c r="AJ47" s="330"/>
-      <c r="AK47" s="330"/>
-      <c r="AL47" s="330"/>
-      <c r="AM47" s="332"/>
+      <c r="AJ47" s="373"/>
+      <c r="AK47" s="373"/>
+      <c r="AL47" s="373"/>
+      <c r="AM47" s="375"/>
     </row>
     <row r="48" spans="1:39" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="333" t="s">
+      <c r="A48" s="376" t="s">
         <v>205</v>
       </c>
       <c r="B48" s="107" t="s">
@@ -7325,57 +7302,57 @@
       <c r="C48" s="107" t="s">
         <v>305</v>
       </c>
-      <c r="F48" s="326"/>
-      <c r="G48" s="326"/>
-      <c r="H48" s="326"/>
-      <c r="I48" s="326"/>
-      <c r="J48" s="326"/>
-      <c r="K48" s="326"/>
-      <c r="L48" s="326">
+      <c r="F48" s="369"/>
+      <c r="G48" s="369"/>
+      <c r="H48" s="369"/>
+      <c r="I48" s="369"/>
+      <c r="J48" s="369"/>
+      <c r="K48" s="369"/>
+      <c r="L48" s="369">
         <v>19000</v>
       </c>
-      <c r="M48" s="327">
+      <c r="M48" s="370">
         <v>27000</v>
       </c>
-      <c r="N48" s="328">
+      <c r="N48" s="371">
         <f>VLOOKUP($C$48,'Haver NA'!$A$1:$J$34,10,0)</f>
         <v>10800</v>
       </c>
-      <c r="O48" s="329">
+      <c r="O48" s="372">
         <v>377.5955484896661</v>
       </c>
-      <c r="P48" s="329">
+      <c r="P48" s="372">
         <v>0</v>
       </c>
-      <c r="Q48" s="329">
+      <c r="Q48" s="372">
         <v>0</v>
       </c>
-      <c r="R48" s="329">
+      <c r="R48" s="372">
         <v>0</v>
       </c>
-      <c r="S48" s="329"/>
-      <c r="T48" s="329"/>
-      <c r="U48" s="329"/>
-      <c r="V48" s="329"/>
-      <c r="W48" s="329"/>
-      <c r="X48" s="329"/>
-      <c r="Y48" s="329"/>
-      <c r="Z48" s="329"/>
-      <c r="AA48" s="329"/>
-      <c r="AB48" s="329"/>
-      <c r="AC48" s="329"/>
-      <c r="AD48" s="329"/>
-      <c r="AE48" s="329"/>
-      <c r="AF48" s="329"/>
-      <c r="AG48" s="329"/>
-      <c r="AI48" s="330"/>
-      <c r="AJ48" s="330"/>
-      <c r="AK48" s="330"/>
-      <c r="AL48" s="330"/>
-      <c r="AM48" s="332"/>
+      <c r="S48" s="372"/>
+      <c r="T48" s="372"/>
+      <c r="U48" s="372"/>
+      <c r="V48" s="372"/>
+      <c r="W48" s="372"/>
+      <c r="X48" s="372"/>
+      <c r="Y48" s="372"/>
+      <c r="Z48" s="372"/>
+      <c r="AA48" s="372"/>
+      <c r="AB48" s="372"/>
+      <c r="AC48" s="372"/>
+      <c r="AD48" s="372"/>
+      <c r="AE48" s="372"/>
+      <c r="AF48" s="372"/>
+      <c r="AG48" s="372"/>
+      <c r="AI48" s="373"/>
+      <c r="AJ48" s="373"/>
+      <c r="AK48" s="373"/>
+      <c r="AL48" s="373"/>
+      <c r="AM48" s="375"/>
     </row>
     <row r="49" spans="1:41" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="333" t="s">
+      <c r="A49" s="376" t="s">
         <v>382</v>
       </c>
       <c r="B49" s="107" t="s">
@@ -7384,44 +7361,44 @@
       <c r="C49" s="107" t="s">
         <v>305</v>
       </c>
-      <c r="F49" s="326"/>
-      <c r="G49" s="326"/>
-      <c r="H49" s="326"/>
-      <c r="I49" s="326"/>
-      <c r="J49" s="326"/>
-      <c r="K49" s="326"/>
-      <c r="L49" s="326"/>
-      <c r="M49" s="327"/>
-      <c r="N49" s="328"/>
-      <c r="O49" s="329">
+      <c r="F49" s="369"/>
+      <c r="G49" s="369"/>
+      <c r="H49" s="369"/>
+      <c r="I49" s="369"/>
+      <c r="J49" s="369"/>
+      <c r="K49" s="369"/>
+      <c r="L49" s="369"/>
+      <c r="M49" s="370"/>
+      <c r="N49" s="371"/>
+      <c r="O49" s="372">
         <v>10800</v>
       </c>
-      <c r="P49" s="329"/>
-      <c r="Q49" s="329"/>
-      <c r="R49" s="329"/>
-      <c r="S49" s="329"/>
-      <c r="T49" s="329"/>
-      <c r="U49" s="329"/>
-      <c r="V49" s="329"/>
-      <c r="W49" s="329"/>
-      <c r="X49" s="329"/>
-      <c r="Y49" s="329"/>
-      <c r="Z49" s="329"/>
-      <c r="AA49" s="329"/>
-      <c r="AB49" s="329"/>
-      <c r="AC49" s="329"/>
-      <c r="AD49" s="329"/>
-      <c r="AE49" s="329"/>
-      <c r="AF49" s="329"/>
-      <c r="AG49" s="329"/>
-      <c r="AI49" s="330"/>
-      <c r="AJ49" s="330"/>
-      <c r="AK49" s="330"/>
-      <c r="AL49" s="330"/>
-      <c r="AM49" s="332"/>
+      <c r="P49" s="372"/>
+      <c r="Q49" s="372"/>
+      <c r="R49" s="372"/>
+      <c r="S49" s="372"/>
+      <c r="T49" s="372"/>
+      <c r="U49" s="372"/>
+      <c r="V49" s="372"/>
+      <c r="W49" s="372"/>
+      <c r="X49" s="372"/>
+      <c r="Y49" s="372"/>
+      <c r="Z49" s="372"/>
+      <c r="AA49" s="372"/>
+      <c r="AB49" s="372"/>
+      <c r="AC49" s="372"/>
+      <c r="AD49" s="372"/>
+      <c r="AE49" s="372"/>
+      <c r="AF49" s="372"/>
+      <c r="AG49" s="372"/>
+      <c r="AI49" s="373"/>
+      <c r="AJ49" s="373"/>
+      <c r="AK49" s="373"/>
+      <c r="AL49" s="373"/>
+      <c r="AM49" s="375"/>
     </row>
     <row r="50" spans="1:41" s="107" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="333" t="s">
+      <c r="A50" s="376" t="s">
         <v>383</v>
       </c>
       <c r="B50" s="107" t="s">
@@ -7430,54 +7407,54 @@
       <c r="C50" s="107" t="s">
         <v>306</v>
       </c>
-      <c r="F50" s="326"/>
-      <c r="G50" s="326"/>
-      <c r="H50" s="326"/>
-      <c r="I50" s="326"/>
-      <c r="J50" s="326"/>
-      <c r="K50" s="326"/>
-      <c r="L50" s="326">
+      <c r="F50" s="369"/>
+      <c r="G50" s="369"/>
+      <c r="H50" s="369"/>
+      <c r="I50" s="369"/>
+      <c r="J50" s="369"/>
+      <c r="K50" s="369"/>
+      <c r="L50" s="369">
         <v>160900</v>
       </c>
-      <c r="M50" s="327">
+      <c r="M50" s="370">
         <v>58400</v>
       </c>
-      <c r="N50" s="328">
+      <c r="N50" s="371">
         <f>VLOOKUP($C$50,'Haver NA'!$A$1:$J$34,10,0)</f>
         <v>34500</v>
       </c>
-      <c r="O50" s="329">
+      <c r="O50" s="372">
         <v>43000</v>
       </c>
-      <c r="P50" s="329">
+      <c r="P50" s="372">
         <v>43000</v>
       </c>
-      <c r="Q50" s="329">
+      <c r="Q50" s="372">
         <v>43000</v>
       </c>
-      <c r="R50" s="329">
+      <c r="R50" s="372">
         <v>15000</v>
       </c>
-      <c r="S50" s="329"/>
-      <c r="T50" s="329"/>
-      <c r="U50" s="329"/>
-      <c r="V50" s="329"/>
-      <c r="W50" s="329"/>
-      <c r="X50" s="329"/>
-      <c r="Y50" s="329"/>
-      <c r="Z50" s="329"/>
-      <c r="AA50" s="329"/>
-      <c r="AB50" s="329"/>
-      <c r="AC50" s="329"/>
-      <c r="AD50" s="329"/>
-      <c r="AE50" s="329"/>
-      <c r="AF50" s="329"/>
-      <c r="AG50" s="329"/>
-      <c r="AI50" s="330"/>
-      <c r="AJ50" s="330"/>
-      <c r="AK50" s="330"/>
-      <c r="AL50" s="330"/>
-      <c r="AM50" s="332"/>
+      <c r="S50" s="372"/>
+      <c r="T50" s="372"/>
+      <c r="U50" s="372"/>
+      <c r="V50" s="372"/>
+      <c r="W50" s="372"/>
+      <c r="X50" s="372"/>
+      <c r="Y50" s="372"/>
+      <c r="Z50" s="372"/>
+      <c r="AA50" s="372"/>
+      <c r="AB50" s="372"/>
+      <c r="AC50" s="372"/>
+      <c r="AD50" s="372"/>
+      <c r="AE50" s="372"/>
+      <c r="AF50" s="372"/>
+      <c r="AG50" s="372"/>
+      <c r="AI50" s="373"/>
+      <c r="AJ50" s="373"/>
+      <c r="AK50" s="373"/>
+      <c r="AL50" s="373"/>
+      <c r="AM50" s="375"/>
     </row>
     <row r="51" spans="1:41" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="86" t="s">
@@ -7523,11 +7500,11 @@
         <v>1663323.8025</v>
       </c>
       <c r="P51" s="88">
-        <f t="shared" ref="P51:Q51" si="36">O51*(1+P53)</f>
+        <f t="shared" ref="P51:Q51" si="35">O51*(1+P53)</f>
         <v>1650848.87398125</v>
       </c>
       <c r="Q51" s="88">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>1638467.5074263907</v>
       </c>
       <c r="R51" s="88">
@@ -7535,15 +7512,15 @@
         <v>1663044.5200377863</v>
       </c>
       <c r="S51" s="88">
-        <f t="shared" ref="S51:U51" si="37">R51*(1+S53)</f>
+        <f t="shared" ref="S51:U51" si="36">R51*(1+S53)</f>
         <v>1687990.187838353</v>
       </c>
       <c r="T51" s="88">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>1713310.0406559282</v>
       </c>
       <c r="U51" s="88">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>1739009.691265767</v>
       </c>
       <c r="V51" s="88">
@@ -7569,7 +7546,7 @@
         <v>1657.1332959769102</v>
       </c>
       <c r="AF51" s="45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>1700.8386099494589</v>
       </c>
       <c r="AG51" s="3"/>
@@ -7608,30 +7585,30 @@
         <v>4.3899160317375507E-2</v>
       </c>
       <c r="H52" s="227">
-        <f t="shared" ref="H52:L52" si="38">H51/G51-1</f>
+        <f t="shared" ref="H52:L52" si="37">H51/G51-1</f>
         <v>3.4867401440725754E-3</v>
       </c>
       <c r="I52" s="227">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>3.5163841628156334E-3</v>
       </c>
       <c r="J52" s="227">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>5.2735975988749129E-3</v>
       </c>
       <c r="K52" s="227">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>3.4509222105193249E-2</v>
       </c>
       <c r="L52" s="227">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>4.7166587697893059E-2</v>
       </c>
       <c r="M52" s="227">
         <v>1.2783825552366457E-2</v>
       </c>
       <c r="N52" s="227">
-        <f t="shared" ref="N52" si="39">N51/M51-1</f>
+        <f t="shared" ref="N52" si="38">N51/M51-1</f>
         <v>3.6483389338011207E-3</v>
       </c>
       <c r="O52" s="226"/>
@@ -7792,51 +7769,51 @@
         <v>610536</v>
       </c>
       <c r="O55" s="144">
-        <f t="shared" ref="O55:Z55" si="40">O56+AVERAGE($H$55:$K$55)</f>
+        <f t="shared" ref="O55:Z55" si="39">O56+AVERAGE($H$55:$K$55)</f>
         <v>794083.58333333337</v>
       </c>
       <c r="P55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>794083.58333333337</v>
       </c>
       <c r="Q55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>144083.58333333331</v>
       </c>
       <c r="R55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>122750.25</v>
       </c>
       <c r="S55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>77330.25</v>
       </c>
       <c r="T55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>77330.25</v>
       </c>
       <c r="U55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>77330.25</v>
       </c>
       <c r="V55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>77330.25</v>
       </c>
       <c r="W55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>74830.25</v>
       </c>
       <c r="X55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>74830.25</v>
       </c>
       <c r="Y55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>74830.25</v>
       </c>
       <c r="Z55" s="144">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>74830.25</v>
       </c>
       <c r="AA55" s="44"/>
@@ -7865,7 +7842,7 @@
         <v>1093900</v>
       </c>
       <c r="N56" s="308">
-        <f t="shared" ref="N56" si="41">N58+N59+N64</f>
+        <f t="shared" ref="N56" si="40">N58+N59+N64</f>
         <v>473700</v>
       </c>
       <c r="O56" s="116">
@@ -7873,31 +7850,31 @@
         <v>719253.33333333337</v>
       </c>
       <c r="P56" s="116">
-        <f t="shared" ref="P56:V56" si="42">P58+P59+SUM(P64:P67)</f>
+        <f t="shared" ref="P56:V56" si="41">P58+P59+SUM(P64:P67)</f>
         <v>719253.33333333337</v>
       </c>
       <c r="Q56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>69253.333333333328</v>
       </c>
       <c r="R56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>47920</v>
       </c>
       <c r="S56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>2500</v>
       </c>
       <c r="T56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>2500</v>
       </c>
       <c r="U56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>2500</v>
       </c>
       <c r="V56" s="116">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>2500</v>
       </c>
       <c r="W56" s="44"/>
@@ -8574,31 +8551,31 @@
         <v>227</v>
       </c>
       <c r="F71" s="203">
-        <f t="shared" ref="F71:L71" si="43">F69-F96</f>
+        <f t="shared" ref="F71:L71" si="42">F69-F96</f>
         <v>196851</v>
       </c>
       <c r="G71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>189684</v>
       </c>
       <c r="H71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>192875</v>
       </c>
       <c r="I71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>191507</v>
       </c>
       <c r="J71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>203997</v>
       </c>
       <c r="K71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>204376</v>
       </c>
       <c r="L71" s="203">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>884250</v>
       </c>
       <c r="M71" s="301">
@@ -8655,47 +8632,47 @@
         <v>197738.804</v>
       </c>
       <c r="P72" s="116">
-        <f t="shared" ref="P72:Z72" si="44">O72*(1+P90)</f>
+        <f t="shared" ref="P72:Z72" si="43">O72*(1+P90)</f>
         <v>198529.75921600001</v>
       </c>
       <c r="Q72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>199323.878252864</v>
       </c>
       <c r="R72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>200121.17376587546</v>
       </c>
       <c r="S72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>200921.65846093895</v>
       </c>
       <c r="T72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>201725.34509478271</v>
       </c>
       <c r="U72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>202532.24647516184</v>
       </c>
       <c r="V72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>203342.37546106247</v>
       </c>
       <c r="W72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>204155.74496290673</v>
       </c>
       <c r="X72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>204972.36794275834</v>
       </c>
       <c r="Y72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>205792.25741452936</v>
       </c>
       <c r="Z72" s="116">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>206615.42644418747</v>
       </c>
       <c r="AA72" s="44"/>
@@ -8769,62 +8746,62 @@
       <c r="K74" s="202"/>
       <c r="L74" s="206">
         <f>SUM(L76:L79)</f>
-        <v>118800</v>
+        <v>90400</v>
       </c>
       <c r="M74" s="206">
-        <f t="shared" ref="M74:N74" si="45">SUM(M76:M79)</f>
-        <v>103600</v>
+        <f t="shared" ref="M74:N74" si="44">SUM(M76:M79)</f>
+        <v>87800</v>
       </c>
       <c r="N74" s="206">
+        <f t="shared" si="44"/>
+        <v>87200</v>
+      </c>
+      <c r="O74" s="116">
+        <f t="shared" ref="O74:Z74" si="45">O75+O81</f>
+        <v>177900</v>
+      </c>
+      <c r="P74" s="116">
         <f t="shared" si="45"/>
-        <v>102400</v>
-      </c>
-      <c r="O74" s="116">
-        <f t="shared" ref="O74:Z74" si="46">O75+O81</f>
-        <v>177900</v>
-      </c>
-      <c r="P74" s="116">
-        <f t="shared" si="46"/>
         <v>121000</v>
       </c>
       <c r="Q74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>121000</v>
       </c>
       <c r="R74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>115000</v>
       </c>
       <c r="S74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>109000</v>
       </c>
       <c r="T74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>109000</v>
       </c>
       <c r="U74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>109000</v>
       </c>
       <c r="V74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>109000</v>
       </c>
       <c r="W74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>109000</v>
       </c>
       <c r="X74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>59000</v>
       </c>
       <c r="Y74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>59000</v>
       </c>
       <c r="Z74" s="116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>59000</v>
       </c>
       <c r="AA74" s="116"/>
@@ -8854,47 +8831,47 @@
         <v>118900</v>
       </c>
       <c r="P75" s="116">
-        <f t="shared" ref="P75:Z75" si="47">SUM(P76:P79)</f>
+        <f t="shared" ref="P75:Z75" si="46">SUM(P76:P79)</f>
         <v>62000</v>
       </c>
       <c r="Q75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>62000</v>
       </c>
       <c r="R75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>56000</v>
       </c>
       <c r="S75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>50000</v>
       </c>
       <c r="T75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>50000</v>
       </c>
       <c r="U75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>50000</v>
       </c>
       <c r="V75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>50000</v>
       </c>
       <c r="W75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>50000</v>
       </c>
       <c r="X75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Y75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Z75" s="116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AA75" s="44"/>
@@ -8971,7 +8948,7 @@
       <c r="AM76" s="233"/>
     </row>
     <row r="77" spans="1:39" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="334" t="s">
+      <c r="A77" s="377" t="s">
         <v>381</v>
       </c>
       <c r="B77" s="107" t="s">
@@ -8980,52 +8957,52 @@
       <c r="C77" s="107" t="s">
         <v>378</v>
       </c>
-      <c r="F77" s="335"/>
-      <c r="G77" s="335"/>
-      <c r="H77" s="335"/>
-      <c r="I77" s="326"/>
-      <c r="J77" s="326"/>
-      <c r="K77" s="326"/>
-      <c r="L77" s="326">
+      <c r="F77" s="378"/>
+      <c r="G77" s="378"/>
+      <c r="H77" s="378"/>
+      <c r="I77" s="369"/>
+      <c r="J77" s="369"/>
+      <c r="K77" s="369"/>
+      <c r="L77" s="369">
         <v>28400</v>
       </c>
-      <c r="M77" s="327">
+      <c r="M77" s="370">
         <v>15800</v>
       </c>
-      <c r="N77" s="336">
+      <c r="N77" s="379">
         <v>15200</v>
       </c>
-      <c r="O77" s="337">
+      <c r="O77" s="380">
         <v>18000</v>
       </c>
-      <c r="P77" s="337">
+      <c r="P77" s="380">
         <v>0</v>
       </c>
-      <c r="Q77" s="337">
+      <c r="Q77" s="380">
         <v>0</v>
       </c>
-      <c r="R77" s="337">
+      <c r="R77" s="380">
         <v>0</v>
       </c>
-      <c r="S77" s="330"/>
-      <c r="T77" s="330"/>
-      <c r="U77" s="330"/>
-      <c r="V77" s="330"/>
-      <c r="W77" s="330"/>
-      <c r="X77" s="330"/>
-      <c r="Y77" s="330"/>
-      <c r="Z77" s="330"/>
-      <c r="AA77" s="330"/>
-      <c r="AB77" s="330"/>
-      <c r="AC77" s="330"/>
-      <c r="AD77" s="330"/>
-      <c r="AE77" s="330"/>
-      <c r="AF77" s="330"/>
-      <c r="AG77" s="330"/>
-      <c r="AM77" s="338"/>
+      <c r="S77" s="373"/>
+      <c r="T77" s="373"/>
+      <c r="U77" s="373"/>
+      <c r="V77" s="373"/>
+      <c r="W77" s="373"/>
+      <c r="X77" s="373"/>
+      <c r="Y77" s="373"/>
+      <c r="Z77" s="373"/>
+      <c r="AA77" s="373"/>
+      <c r="AB77" s="373"/>
+      <c r="AC77" s="373"/>
+      <c r="AD77" s="373"/>
+      <c r="AE77" s="373"/>
+      <c r="AF77" s="373"/>
+      <c r="AG77" s="373"/>
+      <c r="AM77" s="381"/>
     </row>
     <row r="78" spans="1:39" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="334" t="s">
+      <c r="A78" s="377" t="s">
         <v>384</v>
       </c>
       <c r="B78" s="107" t="s">
@@ -9034,46 +9011,40 @@
       <c r="C78" s="107" t="s">
         <v>378</v>
       </c>
-      <c r="F78" s="335"/>
-      <c r="G78" s="335"/>
-      <c r="H78" s="335"/>
-      <c r="I78" s="326"/>
-      <c r="J78" s="326"/>
-      <c r="K78" s="326"/>
-      <c r="L78" s="326">
-        <v>28400</v>
-      </c>
-      <c r="M78" s="327">
-        <v>15800</v>
-      </c>
-      <c r="N78" s="336">
-        <v>15200</v>
-      </c>
-      <c r="O78" s="337">
+      <c r="F78" s="378"/>
+      <c r="G78" s="378"/>
+      <c r="H78" s="378"/>
+      <c r="I78" s="369"/>
+      <c r="J78" s="369"/>
+      <c r="K78" s="369"/>
+      <c r="L78" s="369"/>
+      <c r="M78" s="370"/>
+      <c r="N78" s="379"/>
+      <c r="O78" s="380">
         <v>28900</v>
       </c>
-      <c r="P78" s="337"/>
-      <c r="Q78" s="337"/>
-      <c r="R78" s="337"/>
-      <c r="S78" s="330"/>
-      <c r="T78" s="330"/>
-      <c r="U78" s="330"/>
-      <c r="V78" s="330"/>
-      <c r="W78" s="330"/>
-      <c r="X78" s="330"/>
-      <c r="Y78" s="330"/>
-      <c r="Z78" s="330"/>
-      <c r="AA78" s="330"/>
-      <c r="AB78" s="330"/>
-      <c r="AC78" s="330"/>
-      <c r="AD78" s="330"/>
-      <c r="AE78" s="330"/>
-      <c r="AF78" s="330"/>
-      <c r="AG78" s="330"/>
-      <c r="AM78" s="338"/>
+      <c r="P78" s="380"/>
+      <c r="Q78" s="380"/>
+      <c r="R78" s="380"/>
+      <c r="S78" s="373"/>
+      <c r="T78" s="373"/>
+      <c r="U78" s="373"/>
+      <c r="V78" s="373"/>
+      <c r="W78" s="373"/>
+      <c r="X78" s="373"/>
+      <c r="Y78" s="373"/>
+      <c r="Z78" s="373"/>
+      <c r="AA78" s="373"/>
+      <c r="AB78" s="373"/>
+      <c r="AC78" s="373"/>
+      <c r="AD78" s="373"/>
+      <c r="AE78" s="373"/>
+      <c r="AF78" s="373"/>
+      <c r="AG78" s="373"/>
+      <c r="AM78" s="381"/>
     </row>
     <row r="79" spans="1:39" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="334" t="s">
+      <c r="A79" s="377" t="s">
         <v>201</v>
       </c>
       <c r="B79" s="107" t="s">
@@ -9082,52 +9053,52 @@
       <c r="C79" s="107" t="s">
         <v>379</v>
       </c>
-      <c r="F79" s="335"/>
-      <c r="G79" s="335"/>
-      <c r="H79" s="335"/>
-      <c r="I79" s="326"/>
-      <c r="J79" s="326"/>
-      <c r="K79" s="326"/>
-      <c r="L79" s="326">
+      <c r="F79" s="378"/>
+      <c r="G79" s="378"/>
+      <c r="H79" s="378"/>
+      <c r="I79" s="369"/>
+      <c r="J79" s="369"/>
+      <c r="K79" s="369"/>
+      <c r="L79" s="369">
         <v>27000</v>
       </c>
-      <c r="M79" s="327">
+      <c r="M79" s="370">
         <v>27000</v>
       </c>
-      <c r="N79" s="336">
+      <c r="N79" s="379">
         <v>12000</v>
       </c>
-      <c r="O79" s="337">
+      <c r="O79" s="380">
         <v>12000</v>
       </c>
-      <c r="P79" s="337">
+      <c r="P79" s="380">
         <v>12000</v>
       </c>
-      <c r="Q79" s="337">
+      <c r="Q79" s="380">
         <v>12000</v>
       </c>
-      <c r="R79" s="337">
+      <c r="R79" s="380">
         <v>6000</v>
       </c>
-      <c r="S79" s="330"/>
-      <c r="T79" s="330"/>
-      <c r="U79" s="330"/>
-      <c r="V79" s="330"/>
-      <c r="W79" s="330"/>
-      <c r="X79" s="330"/>
-      <c r="Y79" s="330"/>
-      <c r="Z79" s="330"/>
-      <c r="AA79" s="330"/>
-      <c r="AB79" s="330"/>
-      <c r="AC79" s="330"/>
-      <c r="AD79" s="330"/>
-      <c r="AE79" s="330"/>
-      <c r="AF79" s="330"/>
-      <c r="AG79" s="330"/>
-      <c r="AM79" s="338"/>
+      <c r="S79" s="373"/>
+      <c r="T79" s="373"/>
+      <c r="U79" s="373"/>
+      <c r="V79" s="373"/>
+      <c r="W79" s="373"/>
+      <c r="X79" s="373"/>
+      <c r="Y79" s="373"/>
+      <c r="Z79" s="373"/>
+      <c r="AA79" s="373"/>
+      <c r="AB79" s="373"/>
+      <c r="AC79" s="373"/>
+      <c r="AD79" s="373"/>
+      <c r="AE79" s="373"/>
+      <c r="AF79" s="373"/>
+      <c r="AG79" s="373"/>
+      <c r="AM79" s="381"/>
     </row>
     <row r="80" spans="1:39" s="107" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="334" t="s">
+      <c r="A80" s="377" t="s">
         <v>385</v>
       </c>
       <c r="B80" s="107" t="s">
@@ -9136,43 +9107,43 @@
       <c r="C80" s="107" t="s">
         <v>379</v>
       </c>
-      <c r="F80" s="335"/>
-      <c r="G80" s="335"/>
-      <c r="H80" s="335"/>
-      <c r="I80" s="326"/>
-      <c r="J80" s="326"/>
-      <c r="K80" s="326"/>
-      <c r="L80" s="326">
+      <c r="F80" s="378"/>
+      <c r="G80" s="378"/>
+      <c r="H80" s="378"/>
+      <c r="I80" s="369"/>
+      <c r="J80" s="369"/>
+      <c r="K80" s="369"/>
+      <c r="L80" s="369">
         <v>64400</v>
       </c>
-      <c r="M80" s="339">
+      <c r="M80" s="382">
         <v>23400</v>
       </c>
-      <c r="N80" s="336">
+      <c r="N80" s="379">
         <v>13800</v>
       </c>
-      <c r="O80" s="337">
+      <c r="O80" s="380">
         <v>17100</v>
       </c>
-      <c r="P80" s="337"/>
-      <c r="Q80" s="337"/>
-      <c r="R80" s="337"/>
-      <c r="S80" s="330"/>
-      <c r="T80" s="330"/>
-      <c r="U80" s="330"/>
-      <c r="V80" s="330"/>
-      <c r="W80" s="330"/>
-      <c r="X80" s="330"/>
-      <c r="Y80" s="330"/>
-      <c r="Z80" s="330"/>
-      <c r="AA80" s="330"/>
-      <c r="AB80" s="330"/>
-      <c r="AC80" s="330"/>
-      <c r="AD80" s="330"/>
-      <c r="AE80" s="330"/>
-      <c r="AF80" s="330"/>
-      <c r="AG80" s="330"/>
-      <c r="AM80" s="338"/>
+      <c r="P80" s="380"/>
+      <c r="Q80" s="380"/>
+      <c r="R80" s="380"/>
+      <c r="S80" s="373"/>
+      <c r="T80" s="373"/>
+      <c r="U80" s="373"/>
+      <c r="V80" s="373"/>
+      <c r="W80" s="373"/>
+      <c r="X80" s="373"/>
+      <c r="Y80" s="373"/>
+      <c r="Z80" s="373"/>
+      <c r="AA80" s="373"/>
+      <c r="AB80" s="373"/>
+      <c r="AC80" s="373"/>
+      <c r="AD80" s="373"/>
+      <c r="AE80" s="373"/>
+      <c r="AF80" s="373"/>
+      <c r="AG80" s="373"/>
+      <c r="AM80" s="381"/>
     </row>
     <row r="81" spans="1:39" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="220" t="s">
@@ -9192,47 +9163,47 @@
         <v>59000</v>
       </c>
       <c r="P81" s="116">
-        <f t="shared" ref="P81:Z81" si="48">SUM(P82:P85)</f>
+        <f t="shared" ref="P81:Z81" si="47">SUM(P82:P85)</f>
         <v>59000</v>
       </c>
       <c r="Q81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="R81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="S81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="T81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="U81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="V81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="W81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="X81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="Y81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="Z81" s="116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>59000</v>
       </c>
       <c r="AA81" s="116"/>
@@ -9541,62 +9512,62 @@
       </c>
       <c r="L86" s="206">
         <f>L72+L74</f>
-        <v>349750</v>
+        <v>321350</v>
       </c>
       <c r="M86" s="206">
         <f>M72+M74</f>
-        <v>307200</v>
+        <v>291400</v>
       </c>
       <c r="N86" s="308">
         <f>N72+N74</f>
-        <v>299351</v>
+        <v>284151</v>
       </c>
       <c r="O86" s="144">
-        <f t="shared" ref="O86:Z86" si="49">O72+O74</f>
+        <f t="shared" ref="O86:Z86" si="48">O72+O74</f>
         <v>375638.804</v>
       </c>
       <c r="P86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>319529.75921599998</v>
       </c>
       <c r="Q86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>320323.878252864</v>
       </c>
       <c r="R86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>315121.17376587546</v>
       </c>
       <c r="S86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>309921.65846093895</v>
       </c>
       <c r="T86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>310725.34509478271</v>
       </c>
       <c r="U86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>311532.24647516187</v>
       </c>
       <c r="V86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>312342.37546106247</v>
       </c>
       <c r="W86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>313155.7449629067</v>
       </c>
       <c r="X86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>263972.36794275837</v>
       </c>
       <c r="Y86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>264792.25741452933</v>
       </c>
       <c r="Z86" s="144">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>265615.42644418747</v>
       </c>
       <c r="AA86" s="44"/>
@@ -9931,15 +9902,15 @@
         <v>71400</v>
       </c>
       <c r="P92" s="102">
-        <f t="shared" ref="P92:R92" si="50">SUM(P93:P95)</f>
+        <f t="shared" ref="P92:R92" si="49">SUM(P93:P95)</f>
         <v>71400</v>
       </c>
       <c r="Q92" s="102">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>30600</v>
       </c>
       <c r="R92" s="102">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>30600</v>
       </c>
       <c r="S92" s="186"/>
@@ -10145,23 +10116,23 @@
         <v>512193</v>
       </c>
       <c r="O96" s="116">
-        <f t="shared" ref="O96:S96" si="51">O103*0.74</f>
+        <f t="shared" ref="O96:S96" si="50">O103*0.74</f>
         <v>507477.24811825115</v>
       </c>
       <c r="P96" s="116">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>512541.31638321205</v>
       </c>
       <c r="Q96" s="116">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>512541.31638321205</v>
       </c>
       <c r="R96" s="116">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>512541.31638321205</v>
       </c>
       <c r="S96" s="116">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>512541.31638321205</v>
       </c>
       <c r="T96" s="116">
@@ -10223,31 +10194,31 @@
       <c r="B97" s="141"/>
       <c r="E97" s="141"/>
       <c r="F97" s="201">
-        <f t="shared" ref="F97:L97" si="52">F51+F47+F36+F42</f>
+        <f>F51+F47+F36+F42</f>
         <v>1440187</v>
       </c>
       <c r="G97" s="201">
-        <f t="shared" si="52"/>
+        <f>G51+G47+G36+G42</f>
         <v>1503410</v>
       </c>
       <c r="H97" s="201">
-        <f t="shared" si="52"/>
+        <f>H51+H47+H36+H42</f>
         <v>1508652</v>
       </c>
       <c r="I97" s="201">
-        <f t="shared" si="52"/>
+        <f>I51+I47+I36+I42</f>
         <v>1513957</v>
       </c>
       <c r="J97" s="201">
-        <f t="shared" si="52"/>
+        <f>J51+J47+J36+J42</f>
         <v>1521941</v>
       </c>
       <c r="K97" s="201">
-        <f t="shared" si="52"/>
+        <f>K51+K47+K36+K42</f>
         <v>1574462</v>
       </c>
       <c r="L97" s="201">
-        <f t="shared" si="52"/>
+        <f>L51+L47+L36+L42</f>
         <v>3729557.333333333</v>
       </c>
       <c r="M97" s="301">
@@ -10258,51 +10229,51 @@
         <v>2027793</v>
       </c>
       <c r="O97" s="142">
-        <f t="shared" ref="O97:Z97" si="53">O51+O47+O36+O42+O37+O38+O39</f>
+        <f>O51+O47+O36+O42+O37+O38+O39</f>
         <v>3118501.3980484894</v>
       </c>
       <c r="P97" s="142">
-        <f t="shared" si="53"/>
+        <f>P51+P47+P36+P42+P37+P38+P39</f>
         <v>1874848.87398125</v>
       </c>
       <c r="Q97" s="142">
-        <f t="shared" si="53"/>
+        <f>Q51+Q47+Q36+Q42+Q37+Q38+Q39</f>
         <v>1686467.5074263907</v>
       </c>
       <c r="R97" s="142">
-        <f t="shared" si="53"/>
+        <f>R51+R47+R36+R42+R37+R38+R39</f>
         <v>1683044.5200377863</v>
       </c>
       <c r="S97" s="142">
-        <f t="shared" si="53"/>
+        <f>S51+S47+S36+S42+S37+S38+S39</f>
         <v>1687990.187838353</v>
       </c>
       <c r="T97" s="142">
-        <f t="shared" si="53"/>
+        <f>T51+T47+T36+T42+T37+T38+T39</f>
         <v>1713310.0406559282</v>
       </c>
       <c r="U97" s="142">
-        <f t="shared" si="53"/>
+        <f>U51+U47+U36+U42+U37+U38+U39</f>
         <v>1739009.691265767</v>
       </c>
       <c r="V97" s="142">
-        <f t="shared" si="53"/>
+        <f>V51+V47+V36+V42+V37+V38+V39</f>
         <v>1756399.7881784246</v>
       </c>
       <c r="W97" s="142">
-        <f t="shared" si="53"/>
+        <f>W51+W47+W36+W42+W37+W38+W39</f>
         <v>0</v>
       </c>
       <c r="X97" s="142">
-        <f t="shared" si="53"/>
+        <f>X51+X47+X36+X42+X37+X38+X39</f>
         <v>0</v>
       </c>
       <c r="Y97" s="142">
-        <f t="shared" si="53"/>
+        <f>Y51+Y47+Y36+Y42+Y37+Y38+Y39</f>
         <v>0</v>
       </c>
       <c r="Z97" s="142">
-        <f t="shared" si="53"/>
+        <f>Z51+Z47+Z36+Z42+Z37+Z38+Z39</f>
         <v>0</v>
       </c>
       <c r="AM97" s="233"/>
@@ -10327,55 +10298,55 @@
         <v>1328805</v>
       </c>
       <c r="N98" s="310">
-        <f t="shared" ref="N98:Z98" si="54">N96+N35</f>
+        <f>N96+N35</f>
         <v>1372787</v>
       </c>
       <c r="O98" s="143">
-        <f t="shared" si="54"/>
+        <f>O96+O35</f>
         <v>1390610.1625906522</v>
       </c>
       <c r="P98" s="143">
-        <f t="shared" si="54"/>
+        <f>P96+P35</f>
         <v>1418489.158978964</v>
       </c>
       <c r="Q98" s="143">
-        <f t="shared" si="54"/>
+        <f>Q96+Q35</f>
         <v>1441583.4808422038</v>
       </c>
       <c r="R98" s="143">
-        <f t="shared" si="54"/>
+        <f>R96+R35</f>
         <v>1483962.7404801806</v>
       </c>
       <c r="S98" s="143">
-        <f t="shared" si="54"/>
+        <f>S96+S35</f>
         <v>1515727.7827888038</v>
       </c>
       <c r="T98" s="143">
-        <f t="shared" si="54"/>
+        <f>T96+T35</f>
         <v>1506974.123618965</v>
       </c>
       <c r="U98" s="143">
-        <f t="shared" si="54"/>
+        <f>U96+U35</f>
         <v>1540850.5361376633</v>
       </c>
       <c r="V98" s="143">
-        <f t="shared" si="54"/>
+        <f>V96+V35</f>
         <v>1551631.6801380017</v>
       </c>
       <c r="W98" s="143">
-        <f t="shared" si="54"/>
+        <f>W96+W35</f>
         <v>1091537.5543621723</v>
       </c>
       <c r="X98" s="143">
-        <f t="shared" si="54"/>
+        <f>X96+X35</f>
         <v>1102537.0783156503</v>
       </c>
       <c r="Y98" s="143">
-        <f t="shared" si="54"/>
+        <f>Y96+Y35</f>
         <v>1113647.4454798999</v>
       </c>
       <c r="Z98" s="143">
-        <f t="shared" si="54"/>
+        <f>Z96+Z35</f>
         <v>0</v>
       </c>
       <c r="AM98" s="233"/>
@@ -10432,35 +10403,35 @@
         <v>818740</v>
       </c>
       <c r="O100" s="133">
-        <f t="shared" ref="O100:U100" si="55">O101+O103</f>
+        <f t="shared" ref="O100:U100" si="51">O101+O103</f>
         <v>831250.83502466371</v>
       </c>
       <c r="P100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>838457.84744285408</v>
       </c>
       <c r="Q100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>839187.01967747905</v>
       </c>
       <c r="R100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>840286.24682117626</v>
       </c>
       <c r="S100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>841762.8752842095</v>
       </c>
       <c r="T100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>843107.97501111636</v>
       </c>
       <c r="U100" s="133">
-        <f t="shared" si="55"/>
+        <f t="shared" si="51"/>
         <v>844539.45728929248</v>
       </c>
       <c r="V100" s="133">
-        <f t="shared" ref="V100" si="56">V101+V103</f>
+        <f t="shared" ref="V100" si="52">V101+V103</f>
         <v>846032.64138980373</v>
       </c>
       <c r="AM100" s="233"/>
@@ -10470,27 +10441,27 @@
         <v>229</v>
       </c>
       <c r="F101" s="203">
-        <f t="shared" ref="F101:K101" si="57">F100-F103</f>
+        <f t="shared" ref="F101:K101" si="53">F100-F103</f>
         <v>139025</v>
       </c>
       <c r="G101" s="203">
-        <f t="shared" si="57"/>
+        <f t="shared" si="53"/>
         <v>139342</v>
       </c>
       <c r="H101" s="203">
-        <f t="shared" si="57"/>
+        <f t="shared" si="53"/>
         <v>140228</v>
       </c>
       <c r="I101" s="203">
-        <f t="shared" si="57"/>
+        <f t="shared" si="53"/>
         <v>141105</v>
       </c>
       <c r="J101" s="203">
-        <f t="shared" si="57"/>
+        <f t="shared" si="53"/>
         <v>141335</v>
       </c>
       <c r="K101" s="203">
-        <f t="shared" si="57"/>
+        <f t="shared" si="53"/>
         <v>142991</v>
       </c>
       <c r="L101" s="203">
@@ -10509,31 +10480,31 @@
         <v>145470.76999999999</v>
       </c>
       <c r="P101" s="133">
-        <f t="shared" ref="P101:S101" si="58">O101*(1+P113)</f>
+        <f t="shared" ref="P101:S101" si="54">O101*(1+P113)</f>
         <v>145834.44692499997</v>
       </c>
       <c r="Q101" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="54"/>
         <v>146563.61915962494</v>
       </c>
       <c r="R101" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="54"/>
         <v>147662.84630332215</v>
       </c>
       <c r="S101" s="133">
-        <f t="shared" si="58"/>
+        <f t="shared" si="54"/>
         <v>149139.47476635536</v>
       </c>
       <c r="T101" s="133">
-        <f t="shared" ref="T101:V101" si="59">S101*(1+T112)</f>
+        <f t="shared" ref="T101:V101" si="55">S101*(1+T112)</f>
         <v>150484.57449326222</v>
       </c>
       <c r="U101" s="133">
-        <f t="shared" si="59"/>
+        <f t="shared" si="55"/>
         <v>151916.05677143831</v>
       </c>
       <c r="V101" s="133">
-        <f t="shared" si="59"/>
+        <f t="shared" si="55"/>
         <v>153409.24087194959</v>
       </c>
       <c r="AM101" s="233"/>
@@ -10602,23 +10573,23 @@
         <v>692623.40051785414</v>
       </c>
       <c r="R103" s="135">
-        <f t="shared" ref="R103:V103" si="60">Q103*(1+R104)</f>
+        <f t="shared" ref="R103:V103" si="56">Q103*(1+R104)</f>
         <v>692623.40051785414</v>
       </c>
       <c r="S103" s="135">
-        <f t="shared" si="60"/>
+        <f t="shared" si="56"/>
         <v>692623.40051785414</v>
       </c>
       <c r="T103" s="135">
-        <f t="shared" si="60"/>
+        <f t="shared" si="56"/>
         <v>692623.40051785414</v>
       </c>
       <c r="U103" s="135">
-        <f t="shared" si="60"/>
+        <f t="shared" si="56"/>
         <v>692623.40051785414</v>
       </c>
       <c r="V103" s="135">
-        <f t="shared" si="60"/>
+        <f t="shared" si="56"/>
         <v>692623.40051785414</v>
       </c>
       <c r="AD103" s="45">
@@ -10690,38 +10661,38 @@
         <v>221</v>
       </c>
       <c r="F105" s="208">
-        <f t="shared" ref="F105:L105" si="61">F96/F103</f>
+        <f t="shared" ref="F105:L105" si="57">F96/F103</f>
         <v>0.66058231423538405</v>
       </c>
       <c r="G105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.6749214177505789</v>
       </c>
       <c r="H105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.68242012696430432</v>
       </c>
       <c r="I105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.6730637268687778</v>
       </c>
       <c r="J105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.66395699382859508</v>
       </c>
       <c r="K105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.67846773573296415</v>
       </c>
       <c r="L105" s="208">
-        <f t="shared" si="61"/>
+        <f t="shared" si="57"/>
         <v>0.76648081779484256</v>
       </c>
       <c r="M105" s="208">
         <v>0.71094027669909299</v>
       </c>
       <c r="N105" s="208">
-        <f t="shared" ref="N105" si="62">N96/N103</f>
+        <f t="shared" ref="N105" si="58">N96/N103</f>
         <v>0.76034541114436371</v>
       </c>
       <c r="AD105" s="154"/>
@@ -10776,31 +10747,31 @@
         <v>2009.5840333646127</v>
       </c>
       <c r="P106" s="35">
-        <f t="shared" ref="P106:V106" si="63">O106*(1+P108)</f>
+        <f t="shared" ref="P106:V106" si="59">O106*(1+P108)</f>
         <v>2031.5173022625379</v>
       </c>
       <c r="Q106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2046.001536440413</v>
       </c>
       <c r="R106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2056.0370415493694</v>
       </c>
       <c r="S106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2065.9690878427696</v>
       </c>
       <c r="T106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2073.2112049317075</v>
       </c>
       <c r="U106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2077.6599340006264</v>
       </c>
       <c r="V106" s="35">
-        <f t="shared" si="63"/>
+        <f t="shared" si="59"/>
         <v>2079.3152750495265</v>
       </c>
       <c r="AM106" s="233"/>
@@ -10814,27 +10785,27 @@
       <c r="D107" s="35"/>
       <c r="F107" s="200"/>
       <c r="G107" s="200">
-        <f t="shared" ref="G107:L107" si="64">(G106/F106)-1</f>
+        <f t="shared" ref="G107:L107" si="60">(G106/F106)-1</f>
         <v>7.8113264233139468E-3</v>
       </c>
       <c r="H107" s="200">
-        <f t="shared" si="64"/>
+        <f t="shared" si="60"/>
         <v>6.3596164356336526E-3</v>
       </c>
       <c r="I107" s="200">
-        <f t="shared" si="64"/>
+        <f t="shared" si="60"/>
         <v>1.3823747222907468E-3</v>
       </c>
       <c r="J107" s="200">
-        <f t="shared" si="64"/>
+        <f t="shared" si="60"/>
         <v>3.5990731154167399E-3</v>
       </c>
       <c r="K107" s="200">
-        <f t="shared" si="64"/>
+        <f t="shared" si="60"/>
         <v>2.6527805069758159E-3</v>
       </c>
       <c r="L107" s="200">
-        <f t="shared" si="64"/>
+        <f t="shared" si="60"/>
         <v>-1.36697697207252E-2</v>
       </c>
       <c r="M107" s="302">
@@ -10994,19 +10965,19 @@
         <v>0</v>
       </c>
       <c r="P110">
-        <f t="shared" ref="P110:S110" si="65">O110*(1+P113)</f>
+        <f t="shared" ref="P110:S110" si="61">O110*(1+P113)</f>
         <v>0</v>
       </c>
       <c r="Q110">
-        <f t="shared" si="65"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="R110">
-        <f t="shared" si="65"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="S110">
-        <f t="shared" si="65"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="T110">
@@ -11014,11 +10985,11 @@
         <v>0</v>
       </c>
       <c r="U110">
-        <f t="shared" ref="U110:V110" si="66">T110*(1+U112)</f>
+        <f t="shared" ref="U110:V110" si="62">T110*(1+U112)</f>
         <v>0</v>
       </c>
       <c r="V110">
-        <f t="shared" si="66"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="W110"/>
@@ -11039,11 +11010,11 @@
       <c r="I111" s="200"/>
       <c r="J111" s="200"/>
       <c r="K111" s="200">
-        <f t="shared" ref="K111" si="67">(K109/J109)-1</f>
+        <f t="shared" ref="K111" si="63">(K109/J109)-1</f>
         <v>1.0265546788835067E-2</v>
       </c>
       <c r="L111" s="200">
-        <f t="shared" ref="L111" si="68">(L109/K109)-1</f>
+        <f t="shared" ref="L111" si="64">(L109/K109)-1</f>
         <v>-1.9776620759153429E-2</v>
       </c>
       <c r="M111" s="302">
@@ -11155,82 +11126,82 @@
         <v>163</v>
       </c>
       <c r="F114" s="201">
-        <f t="shared" ref="F114:L114" si="69">F100+F46-F96</f>
+        <f>F100+F46-F96</f>
         <v>339220</v>
       </c>
       <c r="G114" s="201">
-        <f t="shared" si="69"/>
+        <f>G100+G46-G96</f>
         <v>334185</v>
       </c>
       <c r="H114" s="201">
-        <f t="shared" si="69"/>
+        <f>H100+H46-H96</f>
         <v>335532</v>
       </c>
       <c r="I114" s="201">
-        <f t="shared" si="69"/>
+        <f>I100+I46-I96</f>
         <v>344546</v>
       </c>
       <c r="J114" s="201">
-        <f t="shared" si="69"/>
+        <f>J100+J46-J96</f>
         <v>349558</v>
       </c>
       <c r="K114" s="201">
-        <f t="shared" si="69"/>
+        <f>K100+K46-K96</f>
         <v>343658</v>
       </c>
       <c r="L114" s="201">
-        <f t="shared" si="69"/>
+        <f>L100+L46-L96</f>
         <v>560584.66666666674</v>
       </c>
       <c r="M114" s="301">
         <v>528408</v>
       </c>
       <c r="N114" s="306">
-        <f t="shared" ref="N114:Y114" si="70">N100+N46-N96</f>
+        <f>N100+N46-N96</f>
         <v>343247</v>
       </c>
       <c r="O114" s="215">
-        <f t="shared" si="70"/>
+        <f>O100+O46-O96</f>
         <v>383773.58690641256</v>
       </c>
       <c r="P114" s="215">
-        <f t="shared" si="70"/>
+        <f>P100+P46-P96</f>
         <v>369916.53105964203</v>
       </c>
       <c r="Q114" s="215">
-        <f t="shared" si="70"/>
+        <f>Q100+Q46-Q96</f>
         <v>370645.703294267</v>
       </c>
       <c r="R114" s="215">
-        <f t="shared" si="70"/>
+        <f>R100+R46-R96</f>
         <v>371744.93043796421</v>
       </c>
       <c r="S114" s="215">
-        <f t="shared" si="70"/>
+        <f>S100+S46-S96</f>
         <v>373221.55890099745</v>
       </c>
       <c r="T114" s="215">
-        <f t="shared" si="70"/>
+        <f>T100+T46-T96</f>
         <v>416124.06265897548</v>
       </c>
       <c r="U114" s="215">
-        <f t="shared" si="70"/>
+        <f>U100+U46-U96</f>
         <v>417555.5449371516</v>
       </c>
       <c r="V114" s="215">
-        <f t="shared" si="70"/>
+        <f>V100+V46-V96</f>
         <v>419048.72903766285</v>
       </c>
       <c r="W114" s="215">
-        <f t="shared" si="70"/>
+        <f>W100+W46-W96</f>
         <v>0</v>
       </c>
       <c r="X114" s="215">
-        <f t="shared" si="70"/>
+        <f>X100+X46-X96</f>
         <v>0</v>
       </c>
       <c r="Y114" s="215">
-        <f t="shared" si="70"/>
+        <f>Y100+Y46-Y96</f>
         <v>0</v>
       </c>
       <c r="AM114" s="233"/>
@@ -11242,31 +11213,31 @@
       <c r="B115" s="141"/>
       <c r="E115" s="141"/>
       <c r="F115" s="201">
-        <f t="shared" ref="F115:L115" si="71">F103-F96</f>
+        <f t="shared" ref="F115:L115" si="65">F103-F96</f>
         <v>200195</v>
       </c>
       <c r="G115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>194843</v>
       </c>
       <c r="H115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>195304</v>
       </c>
       <c r="I115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>203441</v>
       </c>
       <c r="J115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>208223</v>
       </c>
       <c r="K115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>200667</v>
       </c>
       <c r="L115" s="201">
-        <f t="shared" si="71"/>
+        <f t="shared" si="65"/>
         <v>156183</v>
       </c>
       <c r="M115" s="301">
@@ -11277,47 +11248,47 @@
         <v>161439</v>
       </c>
       <c r="O115" s="142">
-        <f t="shared" ref="O115:Y115" si="72">O103-O96</f>
+        <f t="shared" ref="O115:Y115" si="66">O103-O96</f>
         <v>178302.81690641254</v>
       </c>
       <c r="P115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>180082.08413464209</v>
       </c>
       <c r="Q115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>180082.08413464209</v>
       </c>
       <c r="R115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>180082.08413464209</v>
       </c>
       <c r="S115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>180082.08413464209</v>
       </c>
       <c r="T115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>221639.48816571326</v>
       </c>
       <c r="U115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>221639.48816571326</v>
       </c>
       <c r="V115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>221639.48816571326</v>
       </c>
       <c r="W115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="X115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="Y115" s="142">
-        <f t="shared" si="72"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="AM115" s="233"/>
@@ -11329,27 +11300,27 @@
       <c r="C116" s="35"/>
       <c r="D116" s="35"/>
       <c r="F116" s="201">
-        <f t="shared" ref="F116:K116" si="73">F114-F115</f>
+        <f t="shared" ref="F116:K116" si="67">F114-F115</f>
         <v>139025</v>
       </c>
       <c r="G116" s="201">
-        <f t="shared" si="73"/>
+        <f t="shared" si="67"/>
         <v>139342</v>
       </c>
       <c r="H116" s="201">
-        <f t="shared" si="73"/>
+        <f t="shared" si="67"/>
         <v>140228</v>
       </c>
       <c r="I116" s="201">
-        <f t="shared" si="73"/>
+        <f t="shared" si="67"/>
         <v>141105</v>
       </c>
       <c r="J116" s="201">
-        <f t="shared" si="73"/>
+        <f t="shared" si="67"/>
         <v>141335</v>
       </c>
       <c r="K116" s="201">
-        <f t="shared" si="73"/>
+        <f t="shared" si="67"/>
         <v>142991</v>
       </c>
       <c r="L116" s="201">
@@ -11364,47 +11335,47 @@
         <v>181808</v>
       </c>
       <c r="O116" s="142">
-        <f t="shared" ref="O116:Y116" si="74">O114-O115</f>
+        <f t="shared" ref="O116:Y116" si="68">O114-O115</f>
         <v>205470.77000000002</v>
       </c>
       <c r="P116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>189834.44692499994</v>
       </c>
       <c r="Q116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>190563.61915962491</v>
       </c>
       <c r="R116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>191662.84630332212</v>
       </c>
       <c r="S116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>193139.47476635536</v>
       </c>
       <c r="T116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>194484.57449326222</v>
       </c>
       <c r="U116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>195916.05677143834</v>
       </c>
       <c r="V116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>197409.24087194959</v>
       </c>
       <c r="W116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="X116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="Y116" s="142">
-        <f t="shared" si="74"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="AM116" s="256"/>
@@ -12908,50 +12879,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="358" t="s">
+      <c r="A5" s="343" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="359"/>
-      <c r="C5" s="359"/>
-      <c r="D5" s="359"/>
-      <c r="E5" s="359"/>
-      <c r="F5" s="359"/>
-      <c r="G5" s="359"/>
-      <c r="H5" s="359"/>
-      <c r="I5" s="359"/>
-      <c r="J5" s="359"/>
-      <c r="K5" s="359"/>
-      <c r="L5" s="359"/>
-      <c r="M5" s="359"/>
-      <c r="N5" s="359"/>
-      <c r="O5" s="359"/>
-      <c r="P5" s="359"/>
-      <c r="Q5" s="359"/>
-      <c r="R5" s="359"/>
-      <c r="S5" s="359"/>
+      <c r="B5" s="344"/>
+      <c r="C5" s="344"/>
+      <c r="D5" s="344"/>
+      <c r="E5" s="344"/>
+      <c r="F5" s="344"/>
+      <c r="G5" s="344"/>
+      <c r="H5" s="344"/>
+      <c r="I5" s="344"/>
+      <c r="J5" s="344"/>
+      <c r="K5" s="344"/>
+      <c r="L5" s="344"/>
+      <c r="M5" s="344"/>
+      <c r="N5" s="344"/>
+      <c r="O5" s="344"/>
+      <c r="P5" s="344"/>
+      <c r="Q5" s="344"/>
+      <c r="R5" s="344"/>
+      <c r="S5" s="344"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="360" t="s">
+      <c r="A6" s="345" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
-      <c r="I6" s="360"/>
-      <c r="J6" s="360"/>
-      <c r="K6" s="360"/>
-      <c r="L6" s="360"/>
-      <c r="M6" s="360"/>
-      <c r="N6" s="360"/>
-      <c r="O6" s="360"/>
-      <c r="P6" s="360"/>
-      <c r="Q6" s="360"/>
-      <c r="R6" s="360"/>
-      <c r="S6" s="360"/>
+      <c r="B6" s="345"/>
+      <c r="C6" s="345"/>
+      <c r="D6" s="345"/>
+      <c r="E6" s="345"/>
+      <c r="F6" s="345"/>
+      <c r="G6" s="345"/>
+      <c r="H6" s="345"/>
+      <c r="I6" s="345"/>
+      <c r="J6" s="345"/>
+      <c r="K6" s="345"/>
+      <c r="L6" s="345"/>
+      <c r="M6" s="345"/>
+      <c r="N6" s="345"/>
+      <c r="O6" s="345"/>
+      <c r="P6" s="345"/>
+      <c r="Q6" s="345"/>
+      <c r="R6" s="345"/>
+      <c r="S6" s="345"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -12992,8 +12963,8 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="131"/>
-      <c r="R8" s="361"/>
-      <c r="S8" s="362"/>
+      <c r="R8" s="346"/>
+      <c r="S8" s="347"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="130"/>
@@ -13265,10 +13236,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="342" t="s">
+      <c r="A1" s="327" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="342"/>
+      <c r="B1" s="327"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -13276,18 +13247,18 @@
       <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="363" t="s">
+      <c r="Z1" s="348" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="363"/>
-      <c r="AB1" s="363"/>
-      <c r="AC1" s="341"/>
-      <c r="AD1" s="341"/>
-      <c r="AE1" s="341"/>
-      <c r="AF1" s="341"/>
+      <c r="AA1" s="348"/>
+      <c r="AB1" s="348"/>
+      <c r="AC1" s="326"/>
+      <c r="AD1" s="326"/>
+      <c r="AE1" s="326"/>
+      <c r="AF1" s="326"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A2" s="364" t="s">
+      <c r="A2" s="349" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="107"/>
@@ -13296,45 +13267,45 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A3" s="364"/>
+      <c r="A3" s="349"/>
       <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A4" s="364"/>
+      <c r="A4" s="349"/>
       <c r="B4" s="109"/>
       <c r="C4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A5" s="364"/>
+      <c r="A5" s="349"/>
       <c r="B5" s="98"/>
       <c r="C5" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C7" s="354" t="s">
+      <c r="C7" s="339" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="355"/>
-      <c r="E7" s="355"/>
-      <c r="F7" s="356"/>
-      <c r="G7" s="354" t="s">
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="341"/>
+      <c r="G7" s="339" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="355"/>
-      <c r="I7" s="355"/>
-      <c r="J7" s="356"/>
-      <c r="K7" s="354" t="s">
+      <c r="H7" s="340"/>
+      <c r="I7" s="340"/>
+      <c r="J7" s="341"/>
+      <c r="K7" s="339" t="s">
         <v>176</v>
       </c>
-      <c r="L7" s="355"/>
-      <c r="M7" s="355"/>
-      <c r="N7" s="356"/>
+      <c r="L7" s="340"/>
+      <c r="M7" s="340"/>
+      <c r="N7" s="341"/>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
@@ -15216,88 +15187,88 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="370" t="s">
+      <c r="A2" s="350" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="370"/>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
-      <c r="F2" s="370"/>
-      <c r="G2" s="370"/>
-      <c r="H2" s="370"/>
-      <c r="I2" s="370"/>
-      <c r="J2" s="370"/>
+      <c r="B2" s="350"/>
+      <c r="C2" s="350"/>
+      <c r="D2" s="350"/>
+      <c r="E2" s="350"/>
+      <c r="F2" s="350"/>
+      <c r="G2" s="350"/>
+      <c r="H2" s="350"/>
+      <c r="I2" s="350"/>
+      <c r="J2" s="350"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="370" t="s">
+      <c r="A3" s="350" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="370"/>
-      <c r="C3" s="370"/>
-      <c r="D3" s="370"/>
-      <c r="E3" s="370"/>
-      <c r="F3" s="370"/>
-      <c r="G3" s="370"/>
-      <c r="H3" s="370"/>
-      <c r="I3" s="370"/>
-      <c r="J3" s="370"/>
+      <c r="B3" s="350"/>
+      <c r="C3" s="350"/>
+      <c r="D3" s="350"/>
+      <c r="E3" s="350"/>
+      <c r="F3" s="350"/>
+      <c r="G3" s="350"/>
+      <c r="H3" s="350"/>
+      <c r="I3" s="350"/>
+      <c r="J3" s="350"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="371"/>
-      <c r="B4" s="371"/>
-      <c r="C4" s="371"/>
-      <c r="D4" s="371"/>
-      <c r="E4" s="371"/>
-      <c r="F4" s="371"/>
-      <c r="G4" s="371"/>
-      <c r="H4" s="371"/>
-      <c r="I4" s="371"/>
-      <c r="J4" s="371"/>
-      <c r="K4" s="376" t="s">
+      <c r="A4" s="351"/>
+      <c r="B4" s="351"/>
+      <c r="C4" s="351"/>
+      <c r="D4" s="351"/>
+      <c r="E4" s="351"/>
+      <c r="F4" s="351"/>
+      <c r="G4" s="351"/>
+      <c r="H4" s="351"/>
+      <c r="I4" s="351"/>
+      <c r="J4" s="351"/>
+      <c r="K4" s="356" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="376"/>
-      <c r="M4" s="376"/>
-      <c r="N4" s="376"/>
+      <c r="L4" s="356"/>
+      <c r="M4" s="356"/>
+      <c r="N4" s="356"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="372" t="s">
+      <c r="C5" s="352" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="373"/>
-      <c r="E5" s="373"/>
-      <c r="F5" s="373"/>
-      <c r="G5" s="373"/>
-      <c r="H5" s="373"/>
-      <c r="I5" s="373"/>
-      <c r="J5" s="374"/>
+      <c r="D5" s="353"/>
+      <c r="E5" s="353"/>
+      <c r="F5" s="353"/>
+      <c r="G5" s="353"/>
+      <c r="H5" s="353"/>
+      <c r="I5" s="353"/>
+      <c r="J5" s="354"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="375" t="s">
+      <c r="L5" s="355" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="341"/>
-      <c r="N5" s="341"/>
+      <c r="M5" s="326"/>
+      <c r="N5" s="326"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="366">
+      <c r="C6" s="358">
         <v>2020</v>
       </c>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
-      <c r="G6" s="367"/>
-      <c r="H6" s="367"/>
-      <c r="I6" s="367"/>
-      <c r="J6" s="368"/>
+      <c r="D6" s="359"/>
+      <c r="E6" s="359"/>
+      <c r="F6" s="359"/>
+      <c r="G6" s="359"/>
+      <c r="H6" s="359"/>
+      <c r="I6" s="359"/>
+      <c r="J6" s="360"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15735,24 +15706,24 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="K22" s="341" t="s">
+      <c r="K22" s="326" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="341"/>
-      <c r="M22" s="341"/>
-      <c r="N22" s="341"/>
-      <c r="O22" s="341" t="s">
+      <c r="L22" s="326"/>
+      <c r="M22" s="326"/>
+      <c r="N22" s="326"/>
+      <c r="O22" s="326" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="341"/>
-      <c r="Q22" s="341"/>
-      <c r="R22" s="341"/>
-      <c r="S22" s="341" t="s">
+      <c r="P22" s="326"/>
+      <c r="Q22" s="326"/>
+      <c r="R22" s="326"/>
+      <c r="S22" s="326" t="s">
         <v>11</v>
       </c>
-      <c r="T22" s="341"/>
-      <c r="U22" s="341"/>
-      <c r="V22" s="341"/>
+      <c r="T22" s="326"/>
+      <c r="U22" s="326"/>
+      <c r="V22" s="326"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.35">
       <c r="C23" s="67"/>
@@ -15769,12 +15740,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="369" t="s">
+      <c r="K23" s="361" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="369"/>
-      <c r="M23" s="369"/>
-      <c r="N23" s="369"/>
+      <c r="L23" s="361"/>
+      <c r="M23" s="361"/>
+      <c r="N23" s="361"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15943,7 +15914,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I28" s="365" t="s">
+      <c r="I28" s="357" t="s">
         <v>257</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15993,7 +15964,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="365"/>
+      <c r="I29" s="357"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -16041,7 +16012,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="365"/>
+      <c r="I30" s="357"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -16089,7 +16060,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="365"/>
+      <c r="I31" s="357"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -16151,7 +16122,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="365" t="s">
+      <c r="I33" s="357" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -16199,7 +16170,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I34" s="365"/>
+      <c r="I34" s="357"/>
       <c r="J34" t="s">
         <v>258</v>
       </c>
@@ -16436,12 +16407,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -16449,6 +16414,12 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16555,30 +16526,30 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="378" t="s">
+      <c r="E6" s="365" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="378"/>
-      <c r="G6" s="378"/>
-      <c r="H6" s="378"/>
-      <c r="I6" s="378"/>
-      <c r="J6" s="378"/>
-      <c r="K6" s="378"/>
-      <c r="L6" s="378"/>
-      <c r="M6" s="378"/>
-      <c r="N6" s="378"/>
-      <c r="O6" s="378"/>
-      <c r="P6" s="378"/>
-      <c r="Q6" s="378"/>
-      <c r="R6" s="378"/>
+      <c r="F6" s="365"/>
+      <c r="G6" s="365"/>
+      <c r="H6" s="365"/>
+      <c r="I6" s="365"/>
+      <c r="J6" s="365"/>
+      <c r="K6" s="365"/>
+      <c r="L6" s="365"/>
+      <c r="M6" s="365"/>
+      <c r="N6" s="365"/>
+      <c r="O6" s="365"/>
+      <c r="P6" s="365"/>
+      <c r="Q6" s="365"/>
+      <c r="R6" s="365"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="377" t="s">
+      <c r="A7" s="362" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="377"/>
-      <c r="C7" s="377"/>
-      <c r="D7" s="377"/>
+      <c r="B7" s="362"/>
+      <c r="C7" s="362"/>
+      <c r="D7" s="362"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
@@ -16596,11 +16567,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="377" t="s">
+      <c r="B8" s="362" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="377"/>
-      <c r="D8" s="377"/>
+      <c r="C8" s="362"/>
+      <c r="D8" s="362"/>
       <c r="E8" s="42">
         <v>1717.857</v>
       </c>
@@ -16646,11 +16617,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
-      <c r="B9" s="377" t="s">
+      <c r="B9" s="362" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="377"/>
-      <c r="D9" s="377"/>
+      <c r="C9" s="362"/>
+      <c r="D9" s="362"/>
       <c r="E9" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -16696,11 +16667,11 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="36"/>
-      <c r="B10" s="377" t="s">
+      <c r="B10" s="362" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="377"/>
-      <c r="D10" s="377"/>
+      <c r="C10" s="362"/>
+      <c r="D10" s="362"/>
       <c r="E10" s="42">
         <v>230.245</v>
       </c>
@@ -16746,11 +16717,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="377" t="s">
+      <c r="B11" s="362" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="377"/>
-      <c r="D11" s="377"/>
+      <c r="C11" s="362"/>
+      <c r="D11" s="362"/>
       <c r="E11" s="42">
         <v>271.327</v>
       </c>
@@ -16845,10 +16816,10 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="377" t="s">
+      <c r="C13" s="362" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="377"/>
+      <c r="D13" s="362"/>
       <c r="E13" s="42">
         <v>3462.8009999999999</v>
       </c>
@@ -16999,11 +16970,11 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
-      <c r="B19" s="377" t="s">
+      <c r="B19" s="362" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="377"/>
-      <c r="D19" s="377"/>
+      <c r="C19" s="362"/>
+      <c r="D19" s="362"/>
       <c r="E19" s="42">
         <v>1717.857</v>
       </c>
@@ -17062,11 +17033,11 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
-      <c r="B20" s="377" t="s">
+      <c r="B20" s="362" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="377"/>
-      <c r="D20" s="377"/>
+      <c r="C20" s="362"/>
+      <c r="D20" s="362"/>
       <c r="E20" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -17126,11 +17097,11 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="36"/>
-      <c r="B21" s="377" t="s">
+      <c r="B21" s="362" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="377"/>
-      <c r="D21" s="377"/>
+      <c r="C21" s="362"/>
+      <c r="D21" s="362"/>
       <c r="E21" s="42">
         <v>230.245</v>
       </c>
@@ -17189,11 +17160,11 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="36"/>
-      <c r="B22" s="377" t="s">
+      <c r="B22" s="362" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="377"/>
-      <c r="D22" s="377"/>
+      <c r="C22" s="362"/>
+      <c r="D22" s="362"/>
       <c r="E22" s="42">
         <v>271.327</v>
       </c>
@@ -17306,21 +17277,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="379" t="s">
+      <c r="H27" s="363" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="379"/>
-      <c r="J27" s="379"/>
-      <c r="K27" s="379"/>
-      <c r="L27" s="379"/>
-      <c r="M27" s="379"/>
-      <c r="N27" s="379"/>
-      <c r="O27" s="379"/>
-      <c r="P27" s="379"/>
-      <c r="Q27" s="379"/>
-      <c r="R27" s="379"/>
-      <c r="S27" s="379"/>
-      <c r="T27" s="379"/>
+      <c r="I27" s="363"/>
+      <c r="J27" s="363"/>
+      <c r="K27" s="363"/>
+      <c r="L27" s="363"/>
+      <c r="M27" s="363"/>
+      <c r="N27" s="363"/>
+      <c r="O27" s="363"/>
+      <c r="P27" s="363"/>
+      <c r="Q27" s="363"/>
+      <c r="R27" s="363"/>
+      <c r="S27" s="363"/>
+      <c r="T27" s="363"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
@@ -17636,21 +17607,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="380" t="s">
+      <c r="F37" s="364" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="380"/>
-      <c r="H37" s="380"/>
-      <c r="I37" s="380"/>
-      <c r="J37" s="380"/>
-      <c r="K37" s="380"/>
-      <c r="L37" s="380"/>
-      <c r="M37" s="380"/>
-      <c r="N37" s="380"/>
-      <c r="O37" s="380"/>
-      <c r="P37" s="380"/>
-      <c r="Q37" s="380"/>
-      <c r="R37" s="380"/>
+      <c r="G37" s="364"/>
+      <c r="H37" s="364"/>
+      <c r="I37" s="364"/>
+      <c r="J37" s="364"/>
+      <c r="K37" s="364"/>
+      <c r="L37" s="364"/>
+      <c r="M37" s="364"/>
+      <c r="N37" s="364"/>
+      <c r="O37" s="364"/>
+      <c r="P37" s="364"/>
+      <c r="Q37" s="364"/>
+      <c r="R37" s="364"/>
     </row>
     <row r="38" spans="1:18" ht="17" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
@@ -17966,21 +17937,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="379" t="s">
+      <c r="F48" s="363" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="379"/>
-      <c r="H48" s="379"/>
-      <c r="I48" s="379"/>
-      <c r="J48" s="379"/>
-      <c r="K48" s="379"/>
-      <c r="L48" s="379"/>
-      <c r="M48" s="379"/>
-      <c r="N48" s="379"/>
-      <c r="O48" s="379"/>
-      <c r="P48" s="379"/>
-      <c r="Q48" s="379"/>
-      <c r="R48" s="379"/>
+      <c r="G48" s="363"/>
+      <c r="H48" s="363"/>
+      <c r="I48" s="363"/>
+      <c r="J48" s="363"/>
+      <c r="K48" s="363"/>
+      <c r="L48" s="363"/>
+      <c r="M48" s="363"/>
+      <c r="N48" s="363"/>
+      <c r="O48" s="363"/>
+      <c r="P48" s="363"/>
+      <c r="Q48" s="363"/>
+      <c r="R48" s="363"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
@@ -18292,6 +18263,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -18300,12 +18277,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18344,50 +18315,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="358" t="s">
+      <c r="A5" s="343" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="359"/>
-      <c r="C5" s="359"/>
-      <c r="D5" s="359"/>
-      <c r="E5" s="359"/>
-      <c r="F5" s="359"/>
-      <c r="G5" s="359"/>
-      <c r="H5" s="359"/>
-      <c r="I5" s="359"/>
-      <c r="J5" s="359"/>
-      <c r="K5" s="359"/>
-      <c r="L5" s="359"/>
-      <c r="M5" s="359"/>
-      <c r="N5" s="359"/>
-      <c r="O5" s="359"/>
-      <c r="P5" s="359"/>
-      <c r="Q5" s="359"/>
-      <c r="R5" s="359"/>
-      <c r="S5" s="359"/>
+      <c r="B5" s="344"/>
+      <c r="C5" s="344"/>
+      <c r="D5" s="344"/>
+      <c r="E5" s="344"/>
+      <c r="F5" s="344"/>
+      <c r="G5" s="344"/>
+      <c r="H5" s="344"/>
+      <c r="I5" s="344"/>
+      <c r="J5" s="344"/>
+      <c r="K5" s="344"/>
+      <c r="L5" s="344"/>
+      <c r="M5" s="344"/>
+      <c r="N5" s="344"/>
+      <c r="O5" s="344"/>
+      <c r="P5" s="344"/>
+      <c r="Q5" s="344"/>
+      <c r="R5" s="344"/>
+      <c r="S5" s="344"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="360" t="s">
+      <c r="A6" s="345" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
-      <c r="I6" s="360"/>
-      <c r="J6" s="360"/>
-      <c r="K6" s="360"/>
-      <c r="L6" s="360"/>
-      <c r="M6" s="360"/>
-      <c r="N6" s="360"/>
-      <c r="O6" s="360"/>
-      <c r="P6" s="360"/>
-      <c r="Q6" s="360"/>
-      <c r="R6" s="360"/>
-      <c r="S6" s="360"/>
+      <c r="B6" s="345"/>
+      <c r="C6" s="345"/>
+      <c r="D6" s="345"/>
+      <c r="E6" s="345"/>
+      <c r="F6" s="345"/>
+      <c r="G6" s="345"/>
+      <c r="H6" s="345"/>
+      <c r="I6" s="345"/>
+      <c r="J6" s="345"/>
+      <c r="K6" s="345"/>
+      <c r="L6" s="345"/>
+      <c r="M6" s="345"/>
+      <c r="N6" s="345"/>
+      <c r="O6" s="345"/>
+      <c r="P6" s="345"/>
+      <c r="Q6" s="345"/>
+      <c r="R6" s="345"/>
+      <c r="S6" s="345"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -18427,10 +18398,10 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="361" t="s">
+      <c r="R8" s="346" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="362"/>
+      <c r="S8" s="347"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -21301,10 +21272,10 @@
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="381" t="s">
+      <c r="D75" s="366" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="382"/>
+      <c r="E75" s="367"/>
       <c r="F75" s="25">
         <v>-75.135000000000005</v>
       </c>
@@ -22274,23 +22245,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="349" t="s">
+      <c r="A1" s="334" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="350"/>
+      <c r="B1" s="335"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1" s="240"/>
-      <c r="J1" s="357" t="s">
+      <c r="J1" s="342" t="s">
         <v>279</v>
       </c>
-      <c r="V1" s="341"/>
-      <c r="W1" s="341"/>
-      <c r="X1" s="341"/>
-      <c r="Y1" s="341"/>
+      <c r="V1" s="326"/>
+      <c r="W1" s="326"/>
+      <c r="X1" s="326"/>
+      <c r="Y1" s="326"/>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A2" s="351" t="s">
+      <c r="A2" s="336" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="126"/>
@@ -22298,68 +22269,68 @@
         <v>192</v>
       </c>
       <c r="I2" s="241"/>
-      <c r="J2" s="357"/>
+      <c r="J2" s="342"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A3" s="352"/>
+      <c r="A3" s="337"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>193</v>
       </c>
       <c r="I3" s="241"/>
-      <c r="J3" s="357"/>
+      <c r="J3" s="342"/>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A4" s="352"/>
+      <c r="A4" s="337"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A5" s="353"/>
+      <c r="A5" s="338"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="C7" s="354" t="s">
+      <c r="C7" s="339" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="355"/>
-      <c r="E7" s="355"/>
-      <c r="F7" s="356"/>
-      <c r="G7" s="354" t="s">
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="341"/>
+      <c r="G7" s="339" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="355"/>
-      <c r="I7" s="355"/>
-      <c r="J7" s="356"/>
-      <c r="K7" s="354" t="s">
+      <c r="H7" s="340"/>
+      <c r="I7" s="340"/>
+      <c r="J7" s="341"/>
+      <c r="K7" s="339" t="s">
         <v>176</v>
       </c>
-      <c r="L7" s="355"/>
-      <c r="M7" s="355"/>
-      <c r="N7" s="355"/>
-      <c r="O7" s="354" t="s">
+      <c r="L7" s="340"/>
+      <c r="M7" s="340"/>
+      <c r="N7" s="340"/>
+      <c r="O7" s="339" t="s">
         <v>269</v>
       </c>
-      <c r="P7" s="355"/>
-      <c r="Q7" s="355"/>
-      <c r="R7" s="355"/>
-      <c r="S7" s="354" t="s">
+      <c r="P7" s="340"/>
+      <c r="Q7" s="340"/>
+      <c r="R7" s="340"/>
+      <c r="S7" s="339" t="s">
         <v>273</v>
       </c>
-      <c r="T7" s="355"/>
-      <c r="U7" s="355"/>
-      <c r="V7" s="355"/>
-      <c r="W7" s="354" t="s">
+      <c r="T7" s="340"/>
+      <c r="U7" s="340"/>
+      <c r="V7" s="340"/>
+      <c r="W7" s="339" t="s">
         <v>274</v>
       </c>
-      <c r="X7" s="355"/>
-      <c r="Y7" s="355"/>
-      <c r="Z7" s="355"/>
+      <c r="X7" s="340"/>
+      <c r="Y7" s="340"/>
+      <c r="Z7" s="340"/>
       <c r="AA7" s="222" t="s">
         <v>275</v>
       </c>
@@ -26385,15 +26356,15 @@
       <c r="D68" s="100"/>
       <c r="E68" s="218">
         <f>main!L86/1000</f>
-        <v>349.75</v>
+        <v>321.35000000000002</v>
       </c>
       <c r="F68" s="218">
         <f>main!M86/1000</f>
-        <v>307.2</v>
+        <v>291.39999999999998</v>
       </c>
       <c r="G68" s="151">
         <f>main!N86/1000</f>
-        <v>299.351</v>
+        <v>284.15100000000001</v>
       </c>
       <c r="H68" s="218">
         <f>main!O86/1000</f>
@@ -26647,11 +26618,11 @@
       <c r="E71" s="217"/>
       <c r="F71" s="217">
         <f>F68-F69</f>
-        <v>6.5999999999999659</v>
+        <v>-9.2000000000000455</v>
       </c>
       <c r="G71" s="150">
         <f t="shared" ref="G71:K71" si="118">G68-G69</f>
-        <v>-4.6000000000000227</v>
+        <v>-19.800000000000011</v>
       </c>
       <c r="H71" s="217">
         <f t="shared" si="118"/>
@@ -26882,7 +26853,7 @@
       </c>
       <c r="J2" s="102">
         <f>'add-ons calculations'!E68</f>
-        <v>349.75</v>
+        <v>321.35000000000002</v>
       </c>
       <c r="K2" s="102">
         <v>1084.5999999999999</v>
@@ -26938,11 +26909,11 @@
       </c>
       <c r="I3">
         <f t="array" ref="I3:I24">TRANSPOSE('add-ons calculations'!F71:AA71)</f>
-        <v>6.5999999999999659</v>
+        <v>-9.2000000000000455</v>
       </c>
       <c r="J3" s="102">
         <f>'add-ons calculations'!F68</f>
-        <v>307.2</v>
+        <v>291.39999999999998</v>
       </c>
       <c r="K3" s="102">
         <v>775.2</v>
@@ -26990,11 +26961,11 @@
         <v>0.63599999999996726</v>
       </c>
       <c r="I4">
-        <v>-4.6000000000000227</v>
+        <v>-19.800000000000011</v>
       </c>
       <c r="J4" s="151">
         <f>'add-ons calculations'!G68</f>
-        <v>299.351</v>
+        <v>284.15100000000001</v>
       </c>
       <c r="K4" s="102">
         <v>296.39999999999998</v>
@@ -27949,36 +27920,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="D1" s="341" t="s">
+      <c r="D1" s="326" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="341"/>
-      <c r="F1" s="341"/>
-      <c r="G1" s="341"/>
-      <c r="H1" s="341" t="s">
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="326" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="341"/>
-      <c r="J1" s="341"/>
-      <c r="K1" s="341"/>
-      <c r="L1" s="341" t="s">
+      <c r="I1" s="326"/>
+      <c r="J1" s="326"/>
+      <c r="K1" s="326"/>
+      <c r="L1" s="326" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="341"/>
-      <c r="N1" s="341"/>
-      <c r="O1" s="341"/>
-      <c r="P1" s="341" t="s">
+      <c r="M1" s="326"/>
+      <c r="N1" s="326"/>
+      <c r="O1" s="326"/>
+      <c r="P1" s="326" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="341"/>
-      <c r="R1" s="341"/>
-      <c r="S1" s="341"/>
-      <c r="T1" s="341" t="s">
+      <c r="Q1" s="326"/>
+      <c r="R1" s="326"/>
+      <c r="S1" s="326"/>
+      <c r="T1" s="326" t="s">
         <v>265</v>
       </c>
-      <c r="U1" s="341"/>
-      <c r="V1" s="341"/>
-      <c r="W1" s="341"/>
+      <c r="U1" s="326"/>
+      <c r="V1" s="326"/>
+      <c r="W1" s="326"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D2" s="197" t="s">
@@ -28388,22 +28359,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="349" t="s">
+      <c r="A1" s="334" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="350"/>
+      <c r="B1" s="335"/>
       <c r="C1" s="35"/>
       <c r="I1" s="240"/>
-      <c r="J1" s="357" t="s">
+      <c r="J1" s="342" t="s">
         <v>279</v>
       </c>
-      <c r="V1" s="341"/>
-      <c r="W1" s="341"/>
-      <c r="X1" s="341"/>
-      <c r="Y1" s="341"/>
+      <c r="V1" s="326"/>
+      <c r="W1" s="326"/>
+      <c r="X1" s="326"/>
+      <c r="Y1" s="326"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="351" t="s">
+      <c r="A2" s="336" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="126"/>
@@ -28412,20 +28383,20 @@
       </c>
       <c r="H2" s="95"/>
       <c r="I2" s="241"/>
-      <c r="J2" s="357"/>
+      <c r="J2" s="342"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="352"/>
+      <c r="A3" s="337"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>193</v>
       </c>
       <c r="H3" s="95"/>
       <c r="I3" s="241"/>
-      <c r="J3" s="357"/>
+      <c r="J3" s="342"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="352"/>
+      <c r="A4" s="337"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>194</v>
@@ -28435,7 +28406,7 @@
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="353"/>
+      <c r="A5" s="338"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>181</v>
@@ -28450,42 +28421,42 @@
       <c r="J6" s="95"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C7" s="354" t="s">
+      <c r="C7" s="339" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="355"/>
-      <c r="E7" s="355"/>
-      <c r="F7" s="356"/>
-      <c r="G7" s="354" t="s">
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="341"/>
+      <c r="G7" s="339" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="355"/>
-      <c r="I7" s="355"/>
-      <c r="J7" s="356"/>
-      <c r="K7" s="354" t="s">
+      <c r="H7" s="340"/>
+      <c r="I7" s="340"/>
+      <c r="J7" s="341"/>
+      <c r="K7" s="339" t="s">
         <v>176</v>
       </c>
-      <c r="L7" s="355"/>
-      <c r="M7" s="355"/>
-      <c r="N7" s="355"/>
-      <c r="O7" s="354" t="s">
+      <c r="L7" s="340"/>
+      <c r="M7" s="340"/>
+      <c r="N7" s="340"/>
+      <c r="O7" s="339" t="s">
         <v>269</v>
       </c>
-      <c r="P7" s="355"/>
-      <c r="Q7" s="355"/>
-      <c r="R7" s="355"/>
-      <c r="S7" s="354" t="s">
+      <c r="P7" s="340"/>
+      <c r="Q7" s="340"/>
+      <c r="R7" s="340"/>
+      <c r="S7" s="339" t="s">
         <v>273</v>
       </c>
-      <c r="T7" s="355"/>
-      <c r="U7" s="355"/>
-      <c r="V7" s="355"/>
-      <c r="W7" s="354" t="s">
+      <c r="T7" s="340"/>
+      <c r="U7" s="340"/>
+      <c r="V7" s="340"/>
+      <c r="W7" s="339" t="s">
         <v>274</v>
       </c>
-      <c r="X7" s="355"/>
-      <c r="Y7" s="355"/>
-      <c r="Z7" s="355"/>
+      <c r="X7" s="340"/>
+      <c r="Y7" s="340"/>
+      <c r="Z7" s="340"/>
       <c r="AA7" s="222" t="s">
         <v>275</v>
       </c>
@@ -31374,7 +31345,7 @@
       </c>
       <c r="I2" s="259">
         <f t="array" ref="I2:I23">TRANSPOSE('add-ons calculations'!F71:AA71)</f>
-        <v>6.5999999999999659</v>
+        <v>-9.2000000000000455</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -31403,7 +31374,7 @@
         <v>0.63599999999996726</v>
       </c>
       <c r="I3" s="259">
-        <v>-4.6000000000000227</v>
+        <v>-19.800000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -33022,18 +32993,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33254,6 +33225,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -33266,14 +33245,6 @@
     <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>